<commit_message>
Change spd --> spe
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrique\PycharmProjects\YACG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B0320C-DFE9-4328-9518-0F3DEFF51D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886A6F9D-3B61-4B0B-B1F7-AC691AA6EDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
+    <workbookView xWindow="30612" yWindow="3720" windowWidth="23256" windowHeight="12576" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>Still in conception, not all fields may be filled in</t>
+  </si>
+  <si>
+    <t>Spe</t>
   </si>
 </sst>
 </file>
@@ -831,7 +834,7 @@
     <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="93"/>
     <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="92"/>
     <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="91"/>
-    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spd" dataDxfId="90"/>
+    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="90"/>
     <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="89">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
@@ -868,7 +871,7 @@
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Atk]]),0,VLOOKUP(TableCreature[[#This Row],[Atk]],TableValueAtk[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="72">
-      <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Spd]]),0,VLOOKUP(TableCreature[[#This Row],[Spd]],TableValueSpd[],2,FALSE))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="71">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</calculatedColumnFormula>
@@ -1340,7 +1343,7 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1400,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -1550,7 +1553,7 @@
         <v>#N/A</v>
       </c>
       <c r="AA2" s="1" t="e">
-        <f>IF(ISBLANK(TableCreature[[#This Row],[Spd]]),0,VLOOKUP(TableCreature[[#This Row],[Spd]],TableValueSpd[],2,FALSE))</f>
+        <f>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
       <c r="AB2" s="1">

</xml_diff>

<commit_message>
Add flavor text field (#14)
* Implement flavor text

* Small changes

* Fix bug for creatures

* Add flavor texts

* Add field

* Update exe
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrique\PycharmProjects\YACG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8FE97F-0C0F-470E-937C-E3CEFBE91F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADF573A-97B7-4EE6-A173-7A68B3DE5E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>Token?</t>
+  </si>
+  <si>
+    <t>Flavor text</t>
   </si>
 </sst>
 </file>
@@ -341,11 +344,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="102">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
+  <dxfs count="104">
     <dxf>
       <fill>
         <patternFill patternType="lightDown">
@@ -660,6 +659,10 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -706,6 +709,14 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -830,35 +841,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AG2" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
-  <autoFilter ref="A1:AG2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
-  <tableColumns count="33">
-    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="99"/>
-    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="98"/>
-    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="97"/>
-    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="96"/>
-    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="95"/>
-    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="94"/>
-    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="93"/>
-    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="92"/>
-    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="91"/>
-    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+  <autoFilter ref="A1:AH2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
+  <tableColumns count="34">
+    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="101"/>
+    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="100"/>
+    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="94"/>
+    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="93"/>
+    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="92">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="89">
+    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="91">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="88">
+    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="90">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="87">
+    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="89">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="86">
+    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="88">
       <calculatedColumnFormula>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="85"/>
-    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="87"/>
+    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="86"/>
+    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="85"/>
     <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="84"/>
     <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="83"/>
     <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="82"/>
@@ -902,41 +914,41 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="G1:H4" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:M2" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
-  <autoFilter ref="A1:M2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+  <autoFilter ref="A1:N2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="65"/>
     <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="64"/>
     <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="63"/>
@@ -945,11 +957,12 @@
     <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="60"/>
     <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="59"/>
     <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="58"/>
-    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="57"/>
-    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="56"/>
-    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="55"/>
-    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="54"/>
-    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="53">
+    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="53"/>
+    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="52">
       <calculatedColumnFormula>VLOOKUP(TableEffect[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -958,20 +971,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A1:K2" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="41"/>
-    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="40">
+    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="41"/>
+    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="39">
       <calculatedColumnFormula>VLOOKUP(TableTrait[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1037,15 +1050,15 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
     <sortCondition descending="1" ref="C1:C5"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1348,7 +1361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB54C6D3-7FAB-4A2A-98C1-E20D603E5DF3}">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1368,22 +1381,23 @@
     <col min="10" max="13" width="15.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="8.44140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="35.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="70.6640625" style="1" customWidth="1"/>
-    <col min="20" max="23" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.109375" style="1"/>
+    <col min="16" max="16" width="70.77734375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="35.6640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="70.77734375" style="1" customWidth="1"/>
+    <col min="21" max="24" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="33" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1430,61 +1444,64 @@
         <v>84</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -1535,96 +1552,97 @@
       <c r="O2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="2"/>
+      <c r="U2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
-      <c r="X2" s="1" t="e">
+      <c r="X2" s="2"/>
+      <c r="Y2" s="1" t="e">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="Y2" s="1" t="e">
+      <c r="Z2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,VLOOKUP(TableCreature[[#This Row],[Cost (total)]],TableValueCost[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="Z2" s="1" t="e">
+      <c r="AA2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[HP]]),0,VLOOKUP(TableCreature[[#This Row],[HP]],TableValueHP[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AA2" s="1" t="e">
+      <c r="AB2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[Atk]]),0,VLOOKUP(TableCreature[[#This Row],[Atk]],TableValueAtk[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AB2" s="1" t="e">
+      <c r="AC2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AD2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</f>
         <v>35</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AE2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AF2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AG2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AG2" s="1" t="e">
+      <c r="AH2" s="1" t="e">
         <f>VLOOKUP(TableCreature[[#This Row],[Token?]],TableDevStage[],3,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
-  <conditionalFormatting sqref="A2 J2:N2 X2:AG2">
-    <cfRule type="expression" dxfId="23" priority="10">
+  <conditionalFormatting sqref="A2 J2:N2 Y2:AH2">
+    <cfRule type="expression" dxfId="22" priority="10">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1632,7 +1650,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{836D9E53-6903-4E55-A13E-DD3D2B77EB00}">
       <formula1>ListColor</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{C631AB10-2382-4312-BC45-9DB8F840C6A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{C631AB10-2382-4312-BC45-9DB8F840C6A5}">
       <formula1>ListDevStage</formula1>
     </dataValidation>
   </dataValidations>
@@ -1645,7 +1663,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F470F9-CED3-4133-87AA-27762A49DDB4}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1661,15 +1679,16 @@
     <col min="6" max="6" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="63.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="35.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="70.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="1"/>
+    <col min="9" max="9" width="70.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="35.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="70.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1695,22 +1714,25 @@
         <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1735,17 +1757,18 @@
       <c r="H2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="1">
+      <c r="M2" s="2"/>
+      <c r="N2" s="1">
         <f>VLOOKUP(TableEffect[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</f>
         <v>0</v>
       </c>
@@ -1753,41 +1776,41 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="N2">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1798,7 +1821,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{658F9F3D-B09B-403F-9218-B7A3438DF1FB}">
       <formula1>ListEffectType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{29D1E923-B59D-472A-B48F-57D8B4BBB6DD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{29D1E923-B59D-472A-B48F-57D8B4BBB6DD}">
       <formula1>ListDevStage</formula1>
     </dataValidation>
   </dataValidations>
@@ -1905,12 +1928,12 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add sheet for mechanics
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrique\PycharmProjects\YACG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADF573A-97B7-4EE6-A173-7A68B3DE5E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E529F5C-89DC-4E96-9A55-EA16B097AC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
+    <workbookView xWindow="-38520" yWindow="-2955" windowWidth="38640" windowHeight="15720" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
     <sheet name="Effects" sheetId="4" r:id="rId2"/>
     <sheet name="Traits" sheetId="3" r:id="rId3"/>
-    <sheet name="Creatures - Value" sheetId="2" r:id="rId4"/>
-    <sheet name="Misc" sheetId="5" r:id="rId5"/>
+    <sheet name="Mechanics" sheetId="6" r:id="rId4"/>
+    <sheet name="Creatures - Value" sheetId="2" r:id="rId5"/>
+    <sheet name="Misc" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="ListColor" localSheetId="3">TableColor[Color]</definedName>
     <definedName name="ListColor">TableColor[Color]</definedName>
+    <definedName name="ListDevStage" localSheetId="3">TableDevStage[Dev stage]</definedName>
     <definedName name="ListDevStage">TableDevStage[Dev stage]</definedName>
+    <definedName name="ListEffectType" localSheetId="3">TableEffectType[Effect type]</definedName>
     <definedName name="ListEffectType">TableEffectType[Effect type]</definedName>
+    <definedName name="ListTraitType" localSheetId="3">TableTraitType[Trait type]</definedName>
     <definedName name="ListTraitType">TableTraitType[Trait type]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -30,12 +35,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -293,6 +309,21 @@
   </si>
   <si>
     <t>Flavor text</t>
+  </si>
+  <si>
+    <t>MXXX</t>
+  </si>
+  <si>
+    <t>+Atk (token)</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -308,15 +339,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -324,11 +361,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -340,11 +386,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="104">
+  <dxfs count="135">
     <dxf>
       <fill>
         <patternFill patternType="lightDown">
@@ -354,15 +411,22 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -441,6 +505,27 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
@@ -513,6 +598,79 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8C8C8C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -559,6 +717,71 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -841,71 +1064,71 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133">
   <autoFilter ref="A1:AH2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
   <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="101"/>
-    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="100"/>
-    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="92">
+    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="132"/>
+    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="131"/>
+    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="130"/>
+    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="129"/>
+    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="128"/>
+    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="127"/>
+    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="126"/>
+    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="125"/>
+    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="124"/>
+    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="123">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="91">
+    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="122">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="90">
+    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="121">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="89">
+    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="120">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="88">
+    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="119">
       <calculatedColumnFormula>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="87"/>
-    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="86"/>
-    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="85"/>
-    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="84"/>
-    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="83"/>
-    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="82"/>
-    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="81"/>
-    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="80"/>
-    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="79"/>
-    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="78"/>
-    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="77">
+    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="118"/>
+    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="117"/>
+    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="116"/>
+    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="115"/>
+    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="114"/>
+    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="113"/>
+    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="112"/>
+    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="111"/>
+    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="110"/>
+    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="109"/>
+    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="108">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="76">
+    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="107">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,VLOOKUP(TableCreature[[#This Row],[Cost (total)]],TableValueCost[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="75">
+    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="106">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[HP]]),0,VLOOKUP(TableCreature[[#This Row],[HP]],TableValueHP[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="74">
+    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="105">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Atk]]),0,VLOOKUP(TableCreature[[#This Row],[Atk]],TableValueAtk[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="73">
+    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="104">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="72">
+    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="103">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="71">
+    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="102">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="70">
+    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="101">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="69">
+    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="100">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="68">
+    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="99">
       <calculatedColumnFormula>VLOOKUP(TableCreature[[#This Row],[Token?]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -914,55 +1137,70 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+  <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
+    <sortCondition descending="1" ref="C1:C5"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+  <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="41"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="G1:H4" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
   <autoFilter ref="A1:N2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="54"/>
-    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="53"/>
-    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="52">
+    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="91"/>
+    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="90"/>
+    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="89"/>
+    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="88"/>
+    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="87"/>
+    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="86"/>
+    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="85"/>
+    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="84"/>
+    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="83">
       <calculatedColumnFormula>VLOOKUP(TableEffect[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -971,20 +1209,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
   <autoFilter ref="A1:K2" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="42"/>
-    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="41"/>
-    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="80"/>
+    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="74"/>
+    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="72"/>
+    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="71"/>
+    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="70">
       <calculatedColumnFormula>VLOOKUP(TableTrait[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -993,6 +1231,35 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+  <autoFilter ref="A1:O2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O2">
+    <sortCondition descending="1" ref="D1:D2"/>
+  </sortState>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="64"/>
+    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="63"/>
+    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="62"/>
+    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="61"/>
+    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="60"/>
+    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="59"/>
+    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="58"/>
+    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="57"/>
+    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="55"/>
+    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="54"/>
+    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="53">
+      <calculatedColumnFormula>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A3D9C3E-F2A3-44FB-A619-809AD2FF91C2}" name="TableValueCost" displayName="TableValueCost" ref="A1:B2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{0A3D9C3E-F2A3-44FB-A619-809AD2FF91C2}"/>
   <tableColumns count="2">
@@ -1003,7 +1270,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D43A2D6A-D008-4DB7-B5DD-C20DA025F23B}" name="TableValueColor" displayName="TableValueColor" ref="D1:G2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="D1:G2" xr:uid="{D43A2D6A-D008-4DB7-B5DD-C20DA025F23B}"/>
   <tableColumns count="4">
@@ -1016,7 +1283,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8B989991-971D-45B3-B881-5891B15ADD9B}" name="TableValueHP" displayName="TableValueHP" ref="I1:J2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="I1:J2" xr:uid="{8B989991-971D-45B3-B881-5891B15ADD9B}"/>
   <tableColumns count="2">
@@ -1027,7 +1294,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8CCFCB3C-4379-4941-93B9-2C56A7D66AA5}" name="TableValueAtk" displayName="TableValueAtk" ref="L1:M2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="L1:M2" xr:uid="{8CCFCB3C-4379-4941-93B9-2C56A7D66AA5}"/>
   <tableColumns count="2">
@@ -1038,7 +1305,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}" name="TableValueSpd" displayName="TableValueSpd" ref="O1:P2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="O1:P2" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}"/>
   <tableColumns count="2">
@@ -1049,25 +1316,10 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
-    <sortCondition descending="1" ref="C1:C5"/>
-  </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="34"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1105,7 +1357,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1211,7 +1463,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1353,7 +1605,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1613,36 +1865,36 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2 J2:N2 Y2:AH2">
-    <cfRule type="expression" dxfId="22" priority="10">
+    <cfRule type="expression" dxfId="36" priority="10">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1666,7 +1918,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1776,41 +2028,41 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="26" priority="11">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1928,12 +2180,12 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1953,6 +2205,184 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9837E7-63C2-417A-ACE2-FDDEC9DFAE13}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="70.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="1">
+        <f>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="13" priority="32">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:L1">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+      <formula>"Cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+      <formula>"Black"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+      <formula>"Pink"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>"Purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+      <formula>"White"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+      <formula>"Blue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"Green"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+      <formula>"Orange"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+      <formula>"Yellow"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:L2">
+    <cfRule type="containsText" dxfId="3" priority="19" operator="containsText" text="XXX">
+      <formula>NOT(ISERROR(SEARCH("XXX",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="20" operator="containsText" text="XX">
+      <formula>NOT(ISERROR(SEARCH("XX",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="21" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="expression" dxfId="0" priority="22">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{B4C0356F-E9C7-4679-B4CE-F0024A3D64F2}">
+      <formula1>ListDevStage</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:L2" xr:uid="{64EE96BC-123D-4C4A-8182-4115058D4AF0}">
+      <formula1>"XXX,XX,X"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C196E161-DDDF-437F-9366-70D0E59EA547}">
   <dimension ref="A1:P1"/>
   <sheetViews>
@@ -2026,7 +2456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B963F87D-6D03-4FC0-968B-EAA63CF5DBB8}">
   <dimension ref="A1:K11"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add traits to mechanics' sheet
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E529F5C-89DC-4E96-9A55-EA16B097AC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D51421-4EBC-48EB-AB68-3A6A0E804415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2955" windowWidth="38640" windowHeight="15720" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
+    <workbookView xWindow="-38520" yWindow="-2955" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Notes (READ-ONLY FOR TRAITS)</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1253,7 @@
     <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="57"/>
     <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="56"/>
     <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="55"/>
-    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes (READ-ONLY FOR TRAITS)" dataDxfId="54"/>
     <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="53">
       <calculatedColumnFormula>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
@@ -1615,7 +1618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB54C6D3-7FAB-4A2A-98C1-E20D603E5DF3}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2208,9 +2211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9837E7-63C2-417A-ACE2-FDDEC9DFAE13}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2273,7 +2274,7 @@
         <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
Change notes for traits in Mechanics sheet
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D51421-4EBC-48EB-AB68-3A6A0E804415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC54FE57-D10B-4AE4-A9BC-BFA59AA0A10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2955" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -324,9 +324,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Notes (READ-ONLY FOR TRAITS)</t>
   </si>
 </sst>
 </file>
@@ -674,6 +671,10 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -724,10 +725,6 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1140,47 +1137,47 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
     <sortCondition descending="1" ref="C1:C5"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="G1:H4" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1253,8 +1250,8 @@
     <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="57"/>
     <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="56"/>
     <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="55"/>
-    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes (READ-ONLY FOR TRAITS)" dataDxfId="54"/>
-    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="53">
+    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="54">
       <calculatedColumnFormula>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2211,7 +2208,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9837E7-63C2-417A-ACE2-FDDEC9DFAE13}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2274,7 +2273,7 @@
         <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
Change formatting when filling values
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC54FE57-D10B-4AE4-A9BC-BFA59AA0A10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DC16CB-FCAE-4BC7-8A5D-F3AC10BC2643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
+    <workbookView xWindow="-38520" yWindow="-2955" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -318,12 +318,6 @@
   </si>
   <si>
     <t>XXX</t>
-  </si>
-  <si>
-    <t>XX</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
 </sst>
 </file>
@@ -401,81 +395,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="135">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC81"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF96B0DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD6BBEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB3E6"/>
+  <dxfs count="204">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEBFAFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD1F3FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -485,91 +423,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF8C8C8C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC81"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF96B0DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD6BBEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB3E6"/>
+          <bgColor rgb="FFE4E4E4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -579,70 +433,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF8C8C8C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC81"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF96B0DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD6BBEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB3E6"/>
+          <bgColor rgb="FFC2C2C2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -659,7 +450,147 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFB9EDFF"/>
+          <bgColor rgb="FFFFE7F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3EBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2CFF1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF8E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF0C1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFECECEC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE8F3E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEDD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE0B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
         </patternFill>
       </fill>
     </dxf>
@@ -671,8 +602,565 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8C8C8C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8C8C8C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8C8C8C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE0B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE0B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8C8C8C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8C8C8C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -725,6 +1213,10 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1040,16 +1532,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFB9EDFF"/>
-      <color rgb="FFA3E7FF"/>
-      <color rgb="FF89E0FF"/>
-      <color rgb="FF8C8C8C"/>
-      <color rgb="FF6F6F6F"/>
-      <color rgb="FF96B0DE"/>
-      <color rgb="FFB6C8E8"/>
-      <color rgb="FFFFCC81"/>
-      <color rgb="FFFFB3E6"/>
-      <color rgb="FFFF9BDE"/>
+      <color rgb="FFEBFAFF"/>
+      <color rgb="FFD1F3FF"/>
+      <color rgb="FFE4E4E4"/>
+      <color rgb="FFC2C2C2"/>
+      <color rgb="FFFFE7F7"/>
+      <color rgb="FFFFD1F0"/>
+      <color rgb="FFF3EBF9"/>
+      <color rgb="FFE2CFF1"/>
+      <color rgb="FFFFF8E1"/>
+      <color rgb="FFFFF0C1"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1064,71 +1556,71 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="203" dataDxfId="202">
   <autoFilter ref="A1:AH2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
   <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="132"/>
-    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="131"/>
-    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="130"/>
-    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="129"/>
-    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="128"/>
-    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="127"/>
-    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="126"/>
-    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="125"/>
-    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="124"/>
-    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="123">
+    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="201"/>
+    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="200"/>
+    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="199"/>
+    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="198"/>
+    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="197"/>
+    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="196"/>
+    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="195"/>
+    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="194"/>
+    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="193"/>
+    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="192">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="122">
+    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="191">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="121">
+    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="190">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="120">
+    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="189">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="119">
+    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="188">
       <calculatedColumnFormula>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="118"/>
-    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="117"/>
-    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="116"/>
-    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="115"/>
-    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="114"/>
-    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="113"/>
-    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="112"/>
-    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="111"/>
-    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="110"/>
-    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="109"/>
-    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="108">
+    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="187"/>
+    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="186"/>
+    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="185"/>
+    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="184"/>
+    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="183"/>
+    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="182"/>
+    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="181"/>
+    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="180"/>
+    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="179"/>
+    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="178"/>
+    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="177">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="107">
+    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="176">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,VLOOKUP(TableCreature[[#This Row],[Cost (total)]],TableValueCost[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="106">
+    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="175">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[HP]]),0,VLOOKUP(TableCreature[[#This Row],[HP]],TableValueHP[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="105">
+    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="174">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Atk]]),0,VLOOKUP(TableCreature[[#This Row],[Atk]],TableValueAtk[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="104">
+    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="173">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="103">
+    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="172">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="102">
+    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="171">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="101">
+    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="170">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="100">
+    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="169">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="99">
+    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="168">
       <calculatedColumnFormula>VLOOKUP(TableCreature[[#This Row],[Token?]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1137,70 +1629,70 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
   <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
     <sortCondition descending="1" ref="C1:C5"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115">
   <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
   <autoFilter ref="G1:H4" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166">
   <autoFilter ref="A1:N2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="95"/>
-    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="94"/>
-    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="93"/>
-    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="91"/>
-    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="90"/>
-    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="89"/>
-    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="88"/>
-    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="87"/>
-    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="86"/>
-    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="85"/>
-    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="84"/>
-    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="83">
+    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="165"/>
+    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="164"/>
+    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="163"/>
+    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="162"/>
+    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="161"/>
+    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="160"/>
+    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="159"/>
+    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="158"/>
+    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="157"/>
+    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="156"/>
+    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="155"/>
+    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="154"/>
+    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="153"/>
+    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="152">
       <calculatedColumnFormula>VLOOKUP(TableEffect[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1209,20 +1701,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="151" dataDxfId="150">
   <autoFilter ref="A1:K2" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="80"/>
-    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="77"/>
-    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="76"/>
-    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="75"/>
-    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="74"/>
-    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="72"/>
-    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="70">
+    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="149"/>
+    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="143"/>
+    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="141"/>
+    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="140"/>
+    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="139">
       <calculatedColumnFormula>VLOOKUP(TableTrait[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1231,27 +1723,27 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137">
   <autoFilter ref="A1:O2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O2">
     <sortCondition descending="1" ref="D1:D2"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="64"/>
-    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="63"/>
-    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="62"/>
-    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="61"/>
-    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="60"/>
-    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="59"/>
-    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="58"/>
-    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="57"/>
-    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="55"/>
-    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="37"/>
-    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="135"/>
+    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="134"/>
+    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="133"/>
+    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="132"/>
+    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="131"/>
+    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="130"/>
+    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="129"/>
+    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="128"/>
+    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="127"/>
+    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="126"/>
+    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="125"/>
+    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="124"/>
+    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="123"/>
+    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="122">
       <calculatedColumnFormula>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1865,36 +2357,36 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2 J2:N2 Y2:AH2">
-    <cfRule type="expression" dxfId="36" priority="10">
+    <cfRule type="expression" dxfId="60" priority="10">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="7" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="8" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2028,41 +2520,41 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="26" priority="11">
+    <cfRule type="expression" dxfId="50" priority="11">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="5" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="6" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="8" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="10" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="40" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2180,12 +2672,12 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2293,19 +2785,29 @@
         <v>88</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="K2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L2" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="M2" s="2" t="s">
         <v>75</v>
       </c>
@@ -2318,53 +2820,141 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="13" priority="32">
+    <cfRule type="expression" dxfId="37" priority="56">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:L1">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="28" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="29" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="30" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="43" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="44" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="45" operator="equal">
       <formula>"Yellow"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:L2">
-    <cfRule type="containsText" dxfId="3" priority="19" operator="containsText" text="XXX">
-      <formula>NOT(ISERROR(SEARCH("XXX",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="20" operator="containsText" text="XX">
-      <formula>NOT(ISERROR(SEARCH("XX",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="21" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="0" priority="22">
+    <cfRule type="expression" dxfId="27" priority="46">
       <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Implement mechanics and the "Colors Overview" Excel sheet (#16)
* Rename Mechanic --> GameElement

* Fix title name

* Reorder sections

* Remove class field

* Add mechanic id, misc changes

* Rename function, add mechanics

* Add sheet for mechanics

* Add mechanics

* Fix bug for optional fields

* Implement import/export for mechanics

* Reorder fields

* Fix typo

* Add comments

* Add traits to mechanics' sheet

* Change notes for traits in Mechanics sheet

* Change formatting when filling values

* Add ordering to mechanics sheet

* Add colors to traits

* Add mechanic

* Update .exe

* Fix bug where new mechanics' ids would be generated with the wrong prefix

* Remove unused field

* Fix typo

* Update colors

* Update data

* Add mechanics

* Add traits

* Fix bug with quotes in mechanics' names

* Fix bug in loading traits' colors

* Rename excel sheet

* Remove unused imports

* Update .exe

* Remove hardcoded prefixes

* Update .exe
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrique\PycharmProjects\YACG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADF573A-97B7-4EE6-A173-7A68B3DE5E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C69F85B-B1F9-400C-8159-59A733D0E2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
+    <workbookView xWindow="-28920" yWindow="570" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
     <sheet name="Effects" sheetId="4" r:id="rId2"/>
     <sheet name="Traits" sheetId="3" r:id="rId3"/>
-    <sheet name="Creatures - Value" sheetId="2" r:id="rId4"/>
-    <sheet name="Misc" sheetId="5" r:id="rId5"/>
+    <sheet name="Colors Overview" sheetId="6" r:id="rId4"/>
+    <sheet name="Creatures - Value" sheetId="2" r:id="rId5"/>
+    <sheet name="Misc" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="ListColor" localSheetId="3">TableColor[Color]</definedName>
     <definedName name="ListColor">TableColor[Color]</definedName>
+    <definedName name="ListDevStage" localSheetId="3">TableDevStage[Dev stage]</definedName>
     <definedName name="ListDevStage">TableDevStage[Dev stage]</definedName>
+    <definedName name="ListEffectType" localSheetId="3">TableEffectType[Effect type]</definedName>
     <definedName name="ListEffectType">TableEffectType[Effect type]</definedName>
+    <definedName name="ListTraitType" localSheetId="3">TableTraitType[Trait type]</definedName>
     <definedName name="ListTraitType">TableTraitType[Trait type]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -30,12 +35,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -293,6 +309,15 @@
   </si>
   <si>
     <t>Flavor text</t>
+  </si>
+  <si>
+    <t>MXXX</t>
+  </si>
+  <si>
+    <t>+Atk (token)</t>
+  </si>
+  <si>
+    <t>XXX</t>
   </si>
 </sst>
 </file>
@@ -308,15 +333,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -324,11 +355,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -340,11 +380,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="104">
+  <dxfs count="159">
     <dxf>
       <fill>
         <patternFill patternType="lightDown">
@@ -354,64 +405,22 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC81"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF96B0DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD6BBEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB3E6"/>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEBFAFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD1F3FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -426,74 +435,164 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC81"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF96B0DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD6BBEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB3E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2C2C2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4E4E4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE7F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2CFF1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3EBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF0C1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF8E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFECECEC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE8F3E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEDD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF8C8C8C"/>
         </patternFill>
       </fill>
@@ -501,7 +600,70 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFB9EDFF"/>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE0B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEED5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -513,6 +675,173 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8C8C8C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8C8C8C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -559,6 +888,71 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -817,16 +1211,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFB9EDFF"/>
-      <color rgb="FFA3E7FF"/>
-      <color rgb="FF89E0FF"/>
-      <color rgb="FF8C8C8C"/>
-      <color rgb="FF6F6F6F"/>
-      <color rgb="FF96B0DE"/>
-      <color rgb="FFB6C8E8"/>
-      <color rgb="FFFFCC81"/>
-      <color rgb="FFFFB3E6"/>
-      <color rgb="FFFF9BDE"/>
+      <color rgb="FFEBFAFF"/>
+      <color rgb="FFD1F3FF"/>
+      <color rgb="FFE4E4E4"/>
+      <color rgb="FFC2C2C2"/>
+      <color rgb="FFFFE7F7"/>
+      <color rgb="FFFFD1F0"/>
+      <color rgb="FFF3EBF9"/>
+      <color rgb="FFE2CFF1"/>
+      <color rgb="FFFFF8E1"/>
+      <color rgb="FFFFF0C1"/>
     </mruColors>
   </colors>
   <extLst>
@@ -841,71 +1235,71 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="158" dataDxfId="157">
   <autoFilter ref="A1:AH2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
   <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="101"/>
-    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="100"/>
-    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="92">
+    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="156"/>
+    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="155"/>
+    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="154"/>
+    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="153"/>
+    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="152"/>
+    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="151"/>
+    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="150"/>
+    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="149"/>
+    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="148"/>
+    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="147">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="91">
+    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="146">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="90">
+    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="145">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="89">
+    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="144">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="88">
+    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="143">
       <calculatedColumnFormula>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="87"/>
-    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="86"/>
-    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="85"/>
-    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="84"/>
-    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="83"/>
-    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="82"/>
-    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="81"/>
-    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="80"/>
-    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="79"/>
-    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="78"/>
-    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="77">
+    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="142"/>
+    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="141"/>
+    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="140"/>
+    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="139"/>
+    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="138"/>
+    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="137"/>
+    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="136"/>
+    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="135"/>
+    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="134"/>
+    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="133"/>
+    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="132">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="76">
+    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="131">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,VLOOKUP(TableCreature[[#This Row],[Cost (total)]],TableValueCost[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="75">
+    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="130">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[HP]]),0,VLOOKUP(TableCreature[[#This Row],[HP]],TableValueHP[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="74">
+    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="129">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Atk]]),0,VLOOKUP(TableCreature[[#This Row],[Atk]],TableValueAtk[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="73">
+    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="128">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="72">
+    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="127">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="71">
+    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="126">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="70">
+    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="125">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="69">
+    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="124">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="68">
+    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="123">
       <calculatedColumnFormula>VLOOKUP(TableCreature[[#This Row],[Token?]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -914,55 +1308,70 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+  <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
+    <sortCondition descending="1" ref="C1:C5"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+  <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+  <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="65"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
   <autoFilter ref="G1:H4" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
   <autoFilter ref="A1:N2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="54"/>
-    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="53"/>
-    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="52">
+    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="113"/>
+    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="112"/>
+    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="111"/>
+    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="110"/>
+    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="109"/>
+    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="108"/>
+    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="107">
       <calculatedColumnFormula>VLOOKUP(TableEffect[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -971,20 +1380,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
   <autoFilter ref="A1:K2" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="42"/>
-    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="41"/>
-    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="104"/>
+    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="102"/>
+    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="100"/>
+    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="98"/>
+    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="97"/>
+    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="96"/>
+    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="95"/>
+    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="94">
       <calculatedColumnFormula>VLOOKUP(TableTrait[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -993,6 +1402,35 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+  <autoFilter ref="A1:O2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O2">
+    <sortCondition descending="1" ref="D1:D2"/>
+  </sortState>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="88"/>
+    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="87"/>
+    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="86"/>
+    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="85"/>
+    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="84"/>
+    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="83"/>
+    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="82"/>
+    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="81"/>
+    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="79"/>
+    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="78"/>
+    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="77">
+      <calculatedColumnFormula>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A3D9C3E-F2A3-44FB-A619-809AD2FF91C2}" name="TableValueCost" displayName="TableValueCost" ref="A1:B2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{0A3D9C3E-F2A3-44FB-A619-809AD2FF91C2}"/>
   <tableColumns count="2">
@@ -1003,7 +1441,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D43A2D6A-D008-4DB7-B5DD-C20DA025F23B}" name="TableValueColor" displayName="TableValueColor" ref="D1:G2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="D1:G2" xr:uid="{D43A2D6A-D008-4DB7-B5DD-C20DA025F23B}"/>
   <tableColumns count="4">
@@ -1016,7 +1454,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8B989991-971D-45B3-B881-5891B15ADD9B}" name="TableValueHP" displayName="TableValueHP" ref="I1:J2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="I1:J2" xr:uid="{8B989991-971D-45B3-B881-5891B15ADD9B}"/>
   <tableColumns count="2">
@@ -1027,7 +1465,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8CCFCB3C-4379-4941-93B9-2C56A7D66AA5}" name="TableValueAtk" displayName="TableValueAtk" ref="L1:M2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="L1:M2" xr:uid="{8CCFCB3C-4379-4941-93B9-2C56A7D66AA5}"/>
   <tableColumns count="2">
@@ -1038,7 +1476,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}" name="TableValueSpd" displayName="TableValueSpd" ref="O1:P2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="O1:P2" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}"/>
   <tableColumns count="2">
@@ -1049,25 +1487,10 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
-    <sortCondition descending="1" ref="C1:C5"/>
-  </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="34"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1105,7 +1528,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1211,7 +1634,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1353,7 +1776,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1363,41 +1786,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB54C6D3-7FAB-4A2A-98C1-E20D603E5DF3}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="1" customWidth="1"/>
-    <col min="10" max="13" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.44140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="70.77734375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="20.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="35.6640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="70.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="1" customWidth="1"/>
+    <col min="10" max="13" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="70.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="35.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="70.7109375" style="1" customWidth="1"/>
     <col min="21" max="24" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.109375" style="1"/>
+    <col min="25" max="25" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="33" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1501,7 +1924,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -1613,36 +2036,36 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2 J2:N2 Y2:AH2">
-    <cfRule type="expression" dxfId="22" priority="10">
+    <cfRule type="expression" dxfId="60" priority="10">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="7" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="8" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1666,29 +2089,29 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="70.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="35.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="70.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="5" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="70.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="35.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="70.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1732,7 +2155,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1776,41 +2199,41 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="50" priority="11">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="5" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="6" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="8" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="10" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="40" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1840,23 +2263,23 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="60.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="35.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="70.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="70.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1891,7 +2314,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -1928,12 +2351,12 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1953,6 +2376,282 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9837E7-63C2-417A-ACE2-FDDEC9DFAE13}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="70.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="1">
+        <f>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="37" priority="56">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="25" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:L1">
+    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
+      <formula>"Yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="44" operator="equal">
+      <formula>"Orange"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="43" operator="equal">
+      <formula>"Green"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+      <formula>"Blue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
+      <formula>"White"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
+      <formula>"Purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+      <formula>"Pink"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
+      <formula>"Black"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
+      <formula>"Cyan"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="expression" dxfId="0" priority="46">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{B4C0356F-E9C7-4679-B4CE-F0024A3D64F2}">
+      <formula1>ListDevStage</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:L2" xr:uid="{64EE96BC-123D-4C4A-8182-4115058D4AF0}">
+      <formula1>"XXX,XX,X"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C196E161-DDDF-437F-9366-70D0E59EA547}">
   <dimension ref="A1:P1"/>
   <sheetViews>
@@ -1960,23 +2659,23 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2026,7 +2725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B963F87D-6D03-4FC0-968B-EAA63CF5DBB8}">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -2034,23 +2733,23 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="3"/>
-    <col min="5" max="5" width="7.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="3"/>
-    <col min="7" max="7" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="3"/>
+    <col min="5" max="5" width="7.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="3"/>
+    <col min="7" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="72" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="3"/>
-    <col min="10" max="10" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="3"/>
+    <col min="10" max="10" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="3"/>
+    <col min="12" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -2076,7 +2775,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
@@ -2102,7 +2801,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>70</v>
       </c>
@@ -2128,7 +2827,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>77</v>
       </c>
@@ -2154,7 +2853,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>75</v>
       </c>
@@ -2168,32 +2867,32 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E10" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E11" s="3" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Update size of id columns
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C69F85B-B1F9-400C-8159-59A733D0E2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7319EFD-25C7-4838-AD34-AA236AA5646F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="570" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
+    <workbookView xWindow="-28920" yWindow="570" windowWidth="29040" windowHeight="15720" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Showcase creature YAML</t>
   </si>
   <si>
-    <t>CXXX</t>
-  </si>
-  <si>
     <t>ID Trait 1</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>ID Trait 4</t>
   </si>
   <si>
-    <t>EXXX</t>
-  </si>
-  <si>
     <t>Henrique's Idea</t>
   </si>
   <si>
@@ -311,13 +305,22 @@
     <t>Flavor text</t>
   </si>
   <si>
-    <t>MXXX</t>
-  </si>
-  <si>
     <t>+Atk (token)</t>
   </si>
   <si>
     <t>XXX</t>
+  </si>
+  <si>
+    <t>CREXXX</t>
+  </si>
+  <si>
+    <t>EFFXXX</t>
+  </si>
+  <si>
+    <t>TRAXXX</t>
+  </si>
+  <si>
+    <t>MECXXX</t>
   </si>
 </sst>
 </file>
@@ -1786,13 +1789,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB54C6D3-7FAB-4A2A-98C1-E20D603E5DF3}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" customWidth="1"/>
@@ -1846,7 +1849,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -1864,10 +1867,10 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>21</v>
@@ -1879,19 +1882,19 @@
         <v>24</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>12</v>
@@ -1921,12 +1924,12 @@
         <v>19</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1952,9 +1955,9 @@
       <c r="I2" s="2">
         <v>2</v>
       </c>
-      <c r="J2" s="1" t="str">
+      <c r="J2" s="1" t="e">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</f>
-        <v>Subtle</v>
+        <v>#N/A</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</f>
@@ -1970,14 +1973,14 @@
       </c>
       <c r="N2" s="1">
         <f>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>44</v>
@@ -2012,9 +2015,9 @@
         <f>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AD2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</f>
-        <v>35</v>
+        <v>#N/A</v>
       </c>
       <c r="AE2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</f>
@@ -2089,12 +2092,12 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -2137,7 +2140,7 @@
         <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>21</v>
@@ -2149,27 +2152,27 @@
         <v>24</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" s="2">
         <v>7</v>
@@ -2178,17 +2181,17 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="1">
@@ -2265,7 +2268,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="60.7109375" style="1" customWidth="1"/>
@@ -2308,15 +2311,15 @@
         <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -2334,7 +2337,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>41</v>
@@ -2379,13 +2382,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9837E7-63C2-417A-ACE2-FDDEC9DFAE13}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -2444,51 +2447,51 @@
         <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1">
@@ -2686,13 +2689,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" t="s">
-        <v>73</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2763,13 +2766,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>37</v>
@@ -2777,36 +2780,36 @@
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3">
         <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" s="3">
         <v>20</v>
@@ -2815,24 +2818,24 @@
         <v>29</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" s="3">
         <v>10</v>
@@ -2841,24 +2844,24 @@
         <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
Update size in ids columns
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7319EFD-25C7-4838-AD34-AA236AA5646F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04734AA-FE71-47A2-93B9-481C02AF2E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="570" windowWidth="29040" windowHeight="15720" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
@@ -311,16 +311,16 @@
     <t>XXX</t>
   </si>
   <si>
-    <t>CREXXX</t>
-  </si>
-  <si>
-    <t>EFFXXX</t>
-  </si>
-  <si>
-    <t>TRAXXX</t>
-  </si>
-  <si>
-    <t>MECXXX</t>
+    <t>CRE-XXX</t>
+  </si>
+  <si>
+    <t>EFF-XXX</t>
+  </si>
+  <si>
+    <t>TRA-XXX</t>
+  </si>
+  <si>
+    <t>MEC-XXX</t>
   </si>
 </sst>
 </file>
@@ -1795,8 +1795,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
@@ -2092,12 +2091,12 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -2268,7 +2267,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="60.7109375" style="1" customWidth="1"/>
@@ -2388,7 +2387,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Update id structure (#17)
* Change prefixes

* Update ids inside yaml files

* Update size of id columns

* Change id prefixes

* Change ids in cards names

* Change ids in references

* Update size in ids columns

* Update file names
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C69F85B-B1F9-400C-8159-59A733D0E2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04734AA-FE71-47A2-93B9-481C02AF2E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="570" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
+    <workbookView xWindow="-28920" yWindow="570" windowWidth="29040" windowHeight="15720" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Showcase creature YAML</t>
   </si>
   <si>
-    <t>CXXX</t>
-  </si>
-  <si>
     <t>ID Trait 1</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>ID Trait 4</t>
   </si>
   <si>
-    <t>EXXX</t>
-  </si>
-  <si>
     <t>Henrique's Idea</t>
   </si>
   <si>
@@ -311,13 +305,22 @@
     <t>Flavor text</t>
   </si>
   <si>
-    <t>MXXX</t>
-  </si>
-  <si>
     <t>+Atk (token)</t>
   </si>
   <si>
     <t>XXX</t>
+  </si>
+  <si>
+    <t>CRE-XXX</t>
+  </si>
+  <si>
+    <t>EFF-XXX</t>
+  </si>
+  <si>
+    <t>TRA-XXX</t>
+  </si>
+  <si>
+    <t>MEC-XXX</t>
   </si>
 </sst>
 </file>
@@ -1786,14 +1789,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB54C6D3-7FAB-4A2A-98C1-E20D603E5DF3}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
@@ -1846,7 +1848,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -1864,10 +1866,10 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>21</v>
@@ -1879,19 +1881,19 @@
         <v>24</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>12</v>
@@ -1921,12 +1923,12 @@
         <v>19</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1952,9 +1954,9 @@
       <c r="I2" s="2">
         <v>2</v>
       </c>
-      <c r="J2" s="1" t="str">
+      <c r="J2" s="1" t="e">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</f>
-        <v>Subtle</v>
+        <v>#N/A</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</f>
@@ -1970,14 +1972,14 @@
       </c>
       <c r="N2" s="1">
         <f>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>44</v>
@@ -2012,9 +2014,9 @@
         <f>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AD2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</f>
-        <v>35</v>
+        <v>#N/A</v>
       </c>
       <c r="AE2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</f>
@@ -2089,12 +2091,12 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -2137,7 +2139,7 @@
         <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>21</v>
@@ -2149,27 +2151,27 @@
         <v>24</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" s="2">
         <v>7</v>
@@ -2178,17 +2180,17 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="1">
@@ -2265,7 +2267,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="60.7109375" style="1" customWidth="1"/>
@@ -2308,15 +2310,15 @@
         <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -2334,7 +2336,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>41</v>
@@ -2379,13 +2381,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9837E7-63C2-417A-ACE2-FDDEC9DFAE13}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -2444,51 +2446,51 @@
         <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1">
@@ -2686,13 +2688,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" t="s">
-        <v>73</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2763,13 +2765,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>37</v>
@@ -2777,36 +2779,36 @@
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3">
         <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" s="3">
         <v>20</v>
@@ -2815,24 +2817,24 @@
         <v>29</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" s="3">
         <v>10</v>
@@ -2841,24 +2843,24 @@
         <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
Update creatures data to new format
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04734AA-FE71-47A2-93B9-481C02AF2E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304F4E6D-3935-4037-968F-39B862639E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="570" windowWidth="29040" windowHeight="15720" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
@@ -16,18 +16,19 @@
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
     <sheet name="Effects" sheetId="4" r:id="rId2"/>
     <sheet name="Traits" sheetId="3" r:id="rId3"/>
-    <sheet name="Colors Overview" sheetId="6" r:id="rId4"/>
-    <sheet name="Creatures - Value" sheetId="2" r:id="rId5"/>
-    <sheet name="Misc" sheetId="5" r:id="rId6"/>
+    <sheet name="Attack Effects" sheetId="7" r:id="rId4"/>
+    <sheet name="Colors Overview" sheetId="6" r:id="rId5"/>
+    <sheet name="Creatures - Value" sheetId="2" r:id="rId6"/>
+    <sheet name="Misc" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="ListColor" localSheetId="3">TableColor[Color]</definedName>
+    <definedName name="ListColor" localSheetId="4">TableColor[Color]</definedName>
     <definedName name="ListColor">TableColor[Color]</definedName>
-    <definedName name="ListDevStage" localSheetId="3">TableDevStage[Dev stage]</definedName>
+    <definedName name="ListDevStage" localSheetId="4">TableDevStage[Dev stage]</definedName>
     <definedName name="ListDevStage">TableDevStage[Dev stage]</definedName>
-    <definedName name="ListEffectType" localSheetId="3">TableEffectType[Effect type]</definedName>
+    <definedName name="ListEffectType" localSheetId="4">TableEffectType[Effect type]</definedName>
     <definedName name="ListEffectType">TableEffectType[Effect type]</definedName>
-    <definedName name="ListTraitType" localSheetId="3">TableTraitType[Trait type]</definedName>
+    <definedName name="ListTraitType" localSheetId="4">TableTraitType[Trait type]</definedName>
     <definedName name="ListTraitType">TableTraitType[Trait type]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -182,9 +183,6 @@
     <t>Showcase trait YAML</t>
   </si>
   <si>
-    <t>TXXX</t>
-  </si>
-  <si>
     <t>Template creature</t>
   </si>
   <si>
@@ -321,16 +319,61 @@
   </si>
   <si>
     <t>MEC-XXX</t>
+  </si>
+  <si>
+    <t>ID Atk Tec</t>
+  </si>
+  <si>
+    <t>Atk Str</t>
+  </si>
+  <si>
+    <t>Atk Str Effect</t>
+  </si>
+  <si>
+    <t>Atk Str Effect Value</t>
+  </si>
+  <si>
+    <t>Atk Tec</t>
+  </si>
+  <si>
+    <t>Atk Tec Effect</t>
+  </si>
+  <si>
+    <t>Atk Tec Effect Value</t>
+  </si>
+  <si>
+    <t>ATT-XXX</t>
+  </si>
+  <si>
+    <t>Cookie Monster</t>
+  </si>
+  <si>
+    <t>Eat an Oreo</t>
+  </si>
+  <si>
+    <t>Template attack</t>
+  </si>
+  <si>
+    <t>Showcase attack YAML</t>
+  </si>
+  <si>
+    <t>ID Atk Str</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -398,7 +441,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="159">
+  <dxfs count="186">
     <dxf>
       <fill>
         <patternFill patternType="lightDown">
@@ -409,21 +452,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFEBFAFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD1F3FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBFAFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD1F3FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -433,7 +476,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF8C8C8C"/>
+          <bgColor rgb="FFE4E4E4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -453,7 +496,21 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFE4E4E4"/>
+          <bgColor rgb="FF8C8C8C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE7F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -467,14 +524,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFD1F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE7F7"/>
+          <bgColor rgb="FFF3EBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2CFF1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -488,14 +545,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFE2CFF1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF3EBF9"/>
+          <bgColor rgb="FFFFF8E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF0C1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -509,14 +566,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFF0C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF8E1"/>
+          <bgColor rgb="FFECECEC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -530,14 +587,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFECECEC"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -551,20 +608,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFE8F3E1"/>
         </patternFill>
       </fill>
@@ -572,6 +615,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFDEEDD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -579,14 +629,49 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFDEEDD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9EDFF"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -603,35 +688,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFB3E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD6BBEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF96B0DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE0B3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -644,29 +715,29 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC81"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE0B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEED5"/>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -773,6 +844,34 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
@@ -845,6 +944,91 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1145,10 +1329,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -1162,14 +1342,6 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1238,72 +1410,83 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="158" dataDxfId="157">
-  <autoFilter ref="A1:AH2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
-  <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="156"/>
-    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="155"/>
-    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="154"/>
-    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="153"/>
-    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="152"/>
-    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="151"/>
-    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="150"/>
-    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="149"/>
-    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="148"/>
-    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="147">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AO2" totalsRowShown="0" headerRowDxfId="185" dataDxfId="184">
+  <autoFilter ref="A1:AO2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
+  <tableColumns count="41">
+    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="183"/>
+    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="182"/>
+    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="181"/>
+    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="180"/>
+    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="179"/>
+    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="178"/>
+    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="177"/>
+    <tableColumn id="46" xr3:uid="{B53355CF-4D10-414A-853C-90DFAD26068D}" name="Atk Str" dataDxfId="83"/>
+    <tableColumn id="47" xr3:uid="{C906E5A3-1712-48DF-93C0-BC881151C57E}" name="Atk Tec" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="176"/>
+    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="175">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="146">
+    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="174">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="145">
+    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="173">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="144">
+    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="172">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="143">
+    <tableColumn id="42" xr3:uid="{FCE8FFB0-A25C-4332-9148-D1E698B1141E}" name="Atk Str Effect" dataDxfId="85">
+      <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Str]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="41" xr3:uid="{57099D6D-D357-433A-9C7B-03B59203392F}" name="Atk Str Effect Value" dataDxfId="86"/>
+    <tableColumn id="43" xr3:uid="{A46124C8-35A4-4A34-AAA7-C77DEF20B192}" name="Atk Tec Effect" dataDxfId="87">
+      <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Tec]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="37" xr3:uid="{DDB782B7-3741-45E7-A296-44516E8DD74A}" name="Atk Tec Effect Value" dataDxfId="90"/>
+    <tableColumn id="45" xr3:uid="{099F84C7-585A-4B39-97A1-6BA6794D5145}" name="Token?" dataDxfId="84"/>
+    <tableColumn id="48" xr3:uid="{6E8597CE-3227-4CD4-9431-F586DF7BB02D}" name="Value" dataDxfId="81">
       <calculatedColumnFormula>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="142"/>
-    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="141"/>
-    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="140"/>
-    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="139"/>
-    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="138"/>
-    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="137"/>
-    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="136"/>
-    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="135"/>
-    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="134"/>
-    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="133"/>
-    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="132">
+    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="171"/>
+    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="170"/>
+    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="169"/>
+    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="168"/>
+    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="167"/>
+    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="166"/>
+    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="165"/>
+    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="164"/>
+    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="163"/>
+    <tableColumn id="39" xr3:uid="{6B1B591C-CE53-4B4A-9C9C-F299189689D7}" name="ID Atk Str" dataDxfId="89"/>
+    <tableColumn id="40" xr3:uid="{8B59C247-B367-4385-830E-BA42AF90CC0C}" name="ID Atk Tec" dataDxfId="88"/>
+    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="162">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="131">
+    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="161">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,VLOOKUP(TableCreature[[#This Row],[Cost (total)]],TableValueCost[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="130">
+    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="160">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[HP]]),0,VLOOKUP(TableCreature[[#This Row],[HP]],TableValueHP[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="129">
-      <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Atk]]),0,VLOOKUP(TableCreature[[#This Row],[Atk]],TableValueAtk[],2,FALSE))</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="159">
+      <calculatedColumnFormula>IF(ISBLANK(#REF!),0,VLOOKUP(#REF!,TableValueAtk[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="128">
+    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="158">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="127">
+    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="157">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="126">
+    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="156">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="125">
+    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="155">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="124">
+    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="154">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="123">
-      <calculatedColumnFormula>VLOOKUP(TableCreature[[#This Row],[Token?]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
+    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="153">
+      <calculatedColumnFormula>VLOOKUP(#REF!,TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1311,70 +1494,81 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
-  <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
-    <sortCondition descending="1" ref="C1:C5"/>
-  </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}" name="TableValueSpd" displayName="TableValueSpd" ref="O1:P2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="O1:P2" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{70EAA4A7-45C8-47B4-B396-C1BB012C4459}" name="Spd"/>
+    <tableColumn id="2" xr3:uid="{D4251DEB-6809-4B65-9CDC-E6F699CEE4D1}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
-  <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
+  <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
+    <sortCondition descending="1" ref="C1:C5"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
-  <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+  <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
+  <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="95"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
   <autoFilter ref="G1:H4" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="152" dataDxfId="151">
   <autoFilter ref="A1:N2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="113"/>
-    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="112"/>
-    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="111"/>
-    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="110"/>
-    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="109"/>
-    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="108"/>
-    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="107">
+    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="150"/>
+    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="149"/>
+    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="148"/>
+    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="147"/>
+    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="146"/>
+    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="145"/>
+    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="144"/>
+    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="143"/>
+    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="142"/>
+    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="141"/>
+    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="140"/>
+    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="139"/>
+    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="138"/>
+    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="137">
       <calculatedColumnFormula>VLOOKUP(TableEffect[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1383,20 +1577,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135">
   <autoFilter ref="A1:K2" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="104"/>
-    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="101"/>
-    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="99"/>
-    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="98"/>
-    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="97"/>
-    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="96"/>
-    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="95"/>
-    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="94">
+    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="134"/>
+    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="133"/>
+    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="132"/>
+    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="131"/>
+    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="130"/>
+    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="129"/>
+    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="128"/>
+    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="127"/>
+    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="126"/>
+    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="125"/>
+    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="124">
       <calculatedColumnFormula>VLOOKUP(TableTrait[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1405,27 +1599,48 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0FD50C52-5470-4FA1-B963-FCCA8A3AEA14}" name="TableAttack" displayName="TableAttack" ref="A1:J2" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+  <autoFilter ref="A1:J2" xr:uid="{0FD50C52-5470-4FA1-B963-FCCA8A3AEA14}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{302D1D41-67C7-48CF-B669-F1405844081C}" name="ID" dataDxfId="78"/>
+    <tableColumn id="10" xr3:uid="{DAC69B5A-FDB9-4E40-B9DF-D627D52F7026}" name="Order" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{18D1895A-6B8F-4769-905A-7B17388B3841}" name="Name" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{E78EEE3A-A310-4C93-BB56-91C774378558}" name="Description" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{C2498D1A-0522-4022-9828-720277BAEFA0}" name="Value" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{BB71E515-13E4-4082-A3A1-D5CF11AB41BF}" name="Dev stage" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{0A7A2F02-9DDB-46CC-B9E9-6F4043AA6C8E}" name="Dev name" dataDxfId="72"/>
+    <tableColumn id="8" xr3:uid="{1A01A450-5656-4140-92D1-0B7B3AD63520}" name="Summary" dataDxfId="71"/>
+    <tableColumn id="11" xr3:uid="{A56D811E-456F-4EB8-84F6-7E60D2DC5AE0}" name="Notes" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{C5903060-FD83-4888-9AFB-276905D2A13A}" name="Dev stage order" dataDxfId="69">
+      <calculatedColumnFormula>VLOOKUP(TableAttack[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <autoFilter ref="A1:O2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O2">
     <sortCondition descending="1" ref="D1:D2"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="88"/>
-    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="87"/>
-    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="86"/>
-    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="85"/>
-    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="84"/>
-    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="83"/>
-    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="82"/>
-    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="81"/>
-    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="80"/>
-    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="79"/>
-    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="78"/>
-    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="77">
+    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="118"/>
+    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="117"/>
+    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="116"/>
+    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="115"/>
+    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="114"/>
+    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="113"/>
+    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="112"/>
+    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="111"/>
+    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="110"/>
+    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="109"/>
+    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="108"/>
+    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="107">
       <calculatedColumnFormula>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1433,7 +1648,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A3D9C3E-F2A3-44FB-A619-809AD2FF91C2}" name="TableValueCost" displayName="TableValueCost" ref="A1:B2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{0A3D9C3E-F2A3-44FB-A619-809AD2FF91C2}"/>
   <tableColumns count="2">
@@ -1444,7 +1659,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D43A2D6A-D008-4DB7-B5DD-C20DA025F23B}" name="TableValueColor" displayName="TableValueColor" ref="D1:G2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="D1:G2" xr:uid="{D43A2D6A-D008-4DB7-B5DD-C20DA025F23B}"/>
   <tableColumns count="4">
@@ -1457,7 +1672,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8B989991-971D-45B3-B881-5891B15ADD9B}" name="TableValueHP" displayName="TableValueHP" ref="I1:J2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="I1:J2" xr:uid="{8B989991-971D-45B3-B881-5891B15ADD9B}"/>
   <tableColumns count="2">
@@ -1468,23 +1683,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8CCFCB3C-4379-4941-93B9-2C56A7D66AA5}" name="TableValueAtk" displayName="TableValueAtk" ref="L1:M2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="L1:M2" xr:uid="{8CCFCB3C-4379-4941-93B9-2C56A7D66AA5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{038A2B11-8084-4C2F-A77A-AD359206B6A7}" name="Atk"/>
     <tableColumn id="2" xr3:uid="{1AF63558-B50E-4345-8ED8-AD5D661C3203}" name="Value"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}" name="TableValueSpd" displayName="TableValueSpd" ref="O1:P2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="O1:P2" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{70EAA4A7-45C8-47B4-B396-C1BB012C4459}" name="Spd"/>
-    <tableColumn id="2" xr3:uid="{D4251DEB-6809-4B65-9CDC-E6F699CEE4D1}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1787,10 +1991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB54C6D3-7FAB-4A2A-98C1-E20D603E5DF3}">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,28 +2005,35 @@
     <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" customWidth="1"/>
-    <col min="10" max="13" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="70.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="35.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="70.7109375" style="1" customWidth="1"/>
-    <col min="21" max="24" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="11" max="14" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="70.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="35.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="70.7109375" style="1" customWidth="1"/>
+    <col min="26" max="29" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1845,90 +2056,111 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>72</v>
+      <c r="AO1" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1949,133 +2181,166 @@
         <v>3</v>
       </c>
       <c r="H2" s="2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>2</v>
       </c>
-      <c r="J2" s="1" t="e">
+      <c r="K2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K2" s="1" t="str">
+        <v>Subtle</v>
+      </c>
+      <c r="L2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</f>
         <v/>
       </c>
-      <c r="L2" s="1" t="str">
+      <c r="M2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE))</f>
         <v/>
       </c>
-      <c r="M2" s="1" t="str">
+      <c r="N2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE))</f>
         <v/>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1" t="str">
+        <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Str]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE))</f>
+        <v/>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="1" t="str">
+        <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Tec]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE))</f>
+        <v>Cookie Monster</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="e">
         <f>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="R2" s="2" t="s">
+        <v>#REF!</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="1" t="e">
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF2" s="1" t="e">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="Z2" s="1" t="e">
+      <c r="AG2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,VLOOKUP(TableCreature[[#This Row],[Cost (total)]],TableValueCost[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AA2" s="1" t="e">
+      <c r="AH2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[HP]]),0,VLOOKUP(TableCreature[[#This Row],[HP]],TableValueHP[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AB2" s="1" t="e">
-        <f>IF(ISBLANK(TableCreature[[#This Row],[Atk]]),0,VLOOKUP(TableCreature[[#This Row],[Atk]],TableValueAtk[],2,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC2" s="1" t="e">
+      <c r="AI2" s="1" t="e">
+        <f>IF(ISBLANK(#REF!),0,VLOOKUP(#REF!,TableValueAtk[],2,FALSE))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AJ2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AD2" s="1" t="e">
+      <c r="AK2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AE2" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AM2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AN2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AH2" s="1" t="e">
-        <f>VLOOKUP(TableCreature[[#This Row],[Token?]],TableDevStage[],3,FALSE)</f>
-        <v>#N/A</v>
+      <c r="AO2" s="1" t="e">
+        <f>VLOOKUP(#REF!,TableDevStage[],3,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
-  <conditionalFormatting sqref="A2 J2:N2 Y2:AH2">
-    <cfRule type="expression" dxfId="60" priority="10">
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A2 K2:N2 AF2:AO2">
+    <cfRule type="expression" dxfId="68" priority="13">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="4" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="5" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="6" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="7" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="8" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="10" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="11" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="12" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="Q2">
+    <cfRule type="expression" dxfId="58" priority="3">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="expression" dxfId="56" priority="2">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2">
+    <cfRule type="expression" dxfId="55" priority="1">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{836D9E53-6903-4E55-A13E-DD3D2B77EB00}">
       <formula1>ListColor</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{C631AB10-2382-4312-BC45-9DB8F840C6A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2" xr:uid="{C631AB10-2382-4312-BC45-9DB8F840C6A5}">
       <formula1>ListDevStage</formula1>
     </dataValidation>
   </dataValidations>
@@ -2139,7 +2404,7 @@
         <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>21</v>
@@ -2151,27 +2416,27 @@
         <v>24</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2">
         <v>7</v>
@@ -2180,17 +2445,17 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="1">
@@ -2201,41 +2466,41 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="50" priority="11">
+    <cfRule type="expression" dxfId="54" priority="11">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="2" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="3" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="4" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="5" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="6" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="7" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="8" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="9" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="10" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="40" priority="1">
+    <cfRule type="expression" dxfId="44" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2261,8 +2526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EDC1F1-8E32-4E12-A5F3-D0E3A339A822}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,15 +2575,15 @@
         <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -2336,7 +2601,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>41</v>
@@ -2353,12 +2618,12 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="39" priority="2">
+    <cfRule type="expression" dxfId="43" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="expression" dxfId="38" priority="1">
+    <cfRule type="expression" dxfId="42" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2378,6 +2643,114 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32583BC-C3F7-44B7-9986-764F4DA83BEC}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="9" max="9" width="70.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1">
+        <f>VLOOKUP(TableAttack[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="39" priority="2">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="expression" dxfId="38" priority="1">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{E870C36B-AC30-45BD-82C1-5939FB83ABBB}">
+      <formula1>ListDevStage</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9837E7-63C2-417A-ACE2-FDDEC9DFAE13}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2446,51 +2819,51 @@
         <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1">
@@ -2506,131 +2879,131 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
-      <formula>"X"</formula>
+    <cfRule type="cellIs" dxfId="36" priority="25" operator="equal">
+      <formula>"XXX"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
       <formula>"XX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="25" operator="equal">
-      <formula>"XXX"</formula>
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:L1">
-    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
-      <formula>"Yellow"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="44" operator="equal">
-      <formula>"Orange"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="43" operator="equal">
-      <formula>"Green"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
-      <formula>"Blue"</formula>
+    <cfRule type="cellIs" dxfId="33" priority="28" operator="equal">
+      <formula>"Cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
+      <formula>"Black"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
+      <formula>"Pink"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
+      <formula>"Purple"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
-      <formula>"Purple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
-      <formula>"Pink"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
-      <formula>"Black"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
-      <formula>"Cyan"</formula>
+    <cfRule type="cellIs" dxfId="28" priority="33" operator="equal">
+      <formula>"Blue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="43" operator="equal">
+      <formula>"Green"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="44" operator="equal">
+      <formula>"Orange"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="45" operator="equal">
+      <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
-      <formula>"XXX"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"XX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>"X"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
-      <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
-      <formula>"X"</formula>
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+      <formula>"XXX"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"XX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
-      <formula>"XXX"</formula>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>"X"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"XXX"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"XX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>"XXX"</formula>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
-      <formula>"X"</formula>
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+      <formula>"XXX"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"XX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
-      <formula>"XXX"</formula>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"X"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+      <formula>"XXX"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"XX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"XXX"</formula>
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"X"</formula>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"XXX"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"XX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>"XXX"</formula>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"XX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"X"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
@@ -2653,7 +3026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C196E161-DDDF-437F-9366-70D0E59EA547}">
   <dimension ref="A1:P1"/>
   <sheetViews>
@@ -2688,13 +3061,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>70</v>
-      </c>
-      <c r="G1" t="s">
-        <v>71</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2727,7 +3100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B963F87D-6D03-4FC0-968B-EAA63CF5DBB8}">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -2765,13 +3138,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>37</v>
@@ -2779,36 +3152,36 @@
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="3">
         <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3">
         <v>20</v>
@@ -2817,24 +3190,24 @@
         <v>29</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="3">
         <v>10</v>
@@ -2843,24 +3216,24 @@
         <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
Update to include attacks
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304F4E6D-3935-4037-968F-39B862639E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC9008E-41DF-4DD7-9AAE-748337FF599A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="570" windowWidth="29040" windowHeight="15720" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
     <sheet name="Effects" sheetId="4" r:id="rId2"/>
     <sheet name="Traits" sheetId="3" r:id="rId3"/>
-    <sheet name="Attack Effects" sheetId="7" r:id="rId4"/>
+    <sheet name="Attacks" sheetId="7" r:id="rId4"/>
     <sheet name="Colors Overview" sheetId="6" r:id="rId5"/>
     <sheet name="Creatures - Value" sheetId="2" r:id="rId6"/>
     <sheet name="Misc" sheetId="5" r:id="rId7"/>
@@ -330,18 +330,12 @@
     <t>Atk Str Effect</t>
   </si>
   <si>
-    <t>Atk Str Effect Value</t>
-  </si>
-  <si>
     <t>Atk Tec</t>
   </si>
   <si>
     <t>Atk Tec Effect</t>
   </si>
   <si>
-    <t>Atk Tec Effect Value</t>
-  </si>
-  <si>
     <t>ATT-XXX</t>
   </si>
   <si>
@@ -358,6 +352,12 @@
   </si>
   <si>
     <t>ID Atk Str</t>
+  </si>
+  <si>
+    <t>Atk Str Effect Variable</t>
+  </si>
+  <si>
+    <t>Atk Tec Effect Variable</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="186">
+  <dxfs count="184">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="lightDown">
@@ -450,6 +454,24 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFEBFAFF"/>
@@ -460,13 +482,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFD1F3FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9EDFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -476,7 +491,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFE4E4E4"/>
+          <bgColor rgb="FF8C8C8C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -496,7 +511,21 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF8C8C8C"/>
+          <bgColor rgb="FFE4E4E4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD1F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -510,14 +539,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFD1F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB3E6"/>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2CFF1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -531,14 +560,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFE2CFF1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD6BBEB"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF0C1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -552,14 +581,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFF0C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -573,14 +602,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -601,13 +623,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFE8F3E1"/>
         </patternFill>
       </fill>
@@ -615,6 +630,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFDEEDD3"/>
         </patternFill>
       </fill>
@@ -622,56 +644,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC81"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF96B0DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD6BBEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB3E6"/>
+          <bgColor rgb="FFB9EDFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -688,7 +661,63 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFB9EDFF"/>
+          <bgColor rgb="FFFFB3E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6BBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF96B0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE0B3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -696,34 +725,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE0B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC81"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -865,13 +866,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
@@ -944,91 +938,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1179,6 +1088,51 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1329,6 +1283,30 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -1342,6 +1320,14 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1410,82 +1396,82 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AO2" totalsRowShown="0" headerRowDxfId="185" dataDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AO2" totalsRowShown="0" headerRowDxfId="183" dataDxfId="182">
   <autoFilter ref="A1:AO2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
   <tableColumns count="41">
-    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="183"/>
-    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="182"/>
-    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="181"/>
-    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="180"/>
-    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="179"/>
-    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="178"/>
-    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="177"/>
-    <tableColumn id="46" xr3:uid="{B53355CF-4D10-414A-853C-90DFAD26068D}" name="Atk Str" dataDxfId="83"/>
-    <tableColumn id="47" xr3:uid="{C906E5A3-1712-48DF-93C0-BC881151C57E}" name="Atk Tec" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="176"/>
-    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="175">
+    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="181"/>
+    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="180"/>
+    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="179"/>
+    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="178"/>
+    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="177"/>
+    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="176"/>
+    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="175"/>
+    <tableColumn id="46" xr3:uid="{B53355CF-4D10-414A-853C-90DFAD26068D}" name="Atk Str" dataDxfId="174"/>
+    <tableColumn id="47" xr3:uid="{C906E5A3-1712-48DF-93C0-BC881151C57E}" name="Atk Tec" dataDxfId="173"/>
+    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="172"/>
+    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="171">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="174">
+    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="170">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="173">
+    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="169">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="172">
+    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="168">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{FCE8FFB0-A25C-4332-9148-D1E698B1141E}" name="Atk Str Effect" dataDxfId="85">
+    <tableColumn id="42" xr3:uid="{FCE8FFB0-A25C-4332-9148-D1E698B1141E}" name="Atk Str Effect" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Str]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{57099D6D-D357-433A-9C7B-03B59203392F}" name="Atk Str Effect Value" dataDxfId="86"/>
-    <tableColumn id="43" xr3:uid="{A46124C8-35A4-4A34-AAA7-C77DEF20B192}" name="Atk Tec Effect" dataDxfId="87">
+    <tableColumn id="41" xr3:uid="{57099D6D-D357-433A-9C7B-03B59203392F}" name="Atk Str Effect Variable" dataDxfId="167"/>
+    <tableColumn id="43" xr3:uid="{A46124C8-35A4-4A34-AAA7-C77DEF20B192}" name="Atk Tec Effect" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Tec]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{DDB782B7-3741-45E7-A296-44516E8DD74A}" name="Atk Tec Effect Value" dataDxfId="90"/>
-    <tableColumn id="45" xr3:uid="{099F84C7-585A-4B39-97A1-6BA6794D5145}" name="Token?" dataDxfId="84"/>
-    <tableColumn id="48" xr3:uid="{6E8597CE-3227-4CD4-9431-F586DF7BB02D}" name="Value" dataDxfId="81">
+    <tableColumn id="37" xr3:uid="{DDB782B7-3741-45E7-A296-44516E8DD74A}" name="Atk Tec Effect Variable" dataDxfId="166"/>
+    <tableColumn id="45" xr3:uid="{099F84C7-585A-4B39-97A1-6BA6794D5145}" name="Token?" dataDxfId="165"/>
+    <tableColumn id="48" xr3:uid="{6E8597CE-3227-4CD4-9431-F586DF7BB02D}" name="Value" dataDxfId="164">
       <calculatedColumnFormula>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="171"/>
-    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="170"/>
-    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="169"/>
-    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="168"/>
-    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="167"/>
-    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="166"/>
-    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="165"/>
-    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="164"/>
-    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="163"/>
-    <tableColumn id="39" xr3:uid="{6B1B591C-CE53-4B4A-9C9C-F299189689D7}" name="ID Atk Str" dataDxfId="89"/>
-    <tableColumn id="40" xr3:uid="{8B59C247-B367-4385-830E-BA42AF90CC0C}" name="ID Atk Tec" dataDxfId="88"/>
-    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="162">
+    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="163"/>
+    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="162"/>
+    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="161"/>
+    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="160"/>
+    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="159"/>
+    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="158"/>
+    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="157"/>
+    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="156"/>
+    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="155"/>
+    <tableColumn id="39" xr3:uid="{6B1B591C-CE53-4B4A-9C9C-F299189689D7}" name="ID Atk Str" dataDxfId="154"/>
+    <tableColumn id="40" xr3:uid="{8B59C247-B367-4385-830E-BA42AF90CC0C}" name="ID Atk Tec" dataDxfId="153"/>
+    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="152">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="161">
+    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="151">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,VLOOKUP(TableCreature[[#This Row],[Cost (total)]],TableValueCost[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="160">
+    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="150">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[HP]]),0,VLOOKUP(TableCreature[[#This Row],[HP]],TableValueHP[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="159">
-      <calculatedColumnFormula>IF(ISBLANK(#REF!),0,VLOOKUP(#REF!,TableValueAtk[],2,FALSE))</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="149">
+      <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Atk Str]]),0,VLOOKUP(TableCreature[[#This Row],[Atk Str]],TableValueAtk[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="158">
+    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="148">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="157">
+    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="147">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="156">
+    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="146">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="155">
+    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="145">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="154">
+    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="144">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="153">
+    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="143">
       <calculatedColumnFormula>VLOOKUP(#REF!,TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1505,70 +1491,70 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
   <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
     <sortCondition descending="1" ref="C1:C5"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
   <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="99"/>
+    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="G1:H4" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="152" dataDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141">
   <autoFilter ref="A1:N2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="147"/>
-    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="146"/>
-    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="145"/>
-    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="144"/>
-    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="143"/>
-    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="142"/>
-    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="141"/>
-    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="140"/>
-    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="139"/>
-    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="138"/>
-    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="137">
+    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="140"/>
+    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="139"/>
+    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="138"/>
+    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="137"/>
+    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="136"/>
+    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="135"/>
+    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="134"/>
+    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="133"/>
+    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="132"/>
+    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="131"/>
+    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="130"/>
+    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="129"/>
+    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="128"/>
+    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="127">
       <calculatedColumnFormula>VLOOKUP(TableEffect[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1577,20 +1563,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
   <autoFilter ref="A1:K2" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="134"/>
-    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="133"/>
-    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="132"/>
-    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="131"/>
-    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="130"/>
-    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="129"/>
-    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="128"/>
-    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="127"/>
-    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="126"/>
-    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="125"/>
-    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="124">
+    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="124"/>
+    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="119"/>
+    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="118"/>
+    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="117"/>
+    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="116"/>
+    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="115"/>
+    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="114">
       <calculatedColumnFormula>VLOOKUP(TableTrait[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1599,19 +1585,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0FD50C52-5470-4FA1-B963-FCCA8A3AEA14}" name="TableAttack" displayName="TableAttack" ref="A1:J2" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0FD50C52-5470-4FA1-B963-FCCA8A3AEA14}" name="TableAttack" displayName="TableAttack" ref="A1:J2" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="A1:J2" xr:uid="{0FD50C52-5470-4FA1-B963-FCCA8A3AEA14}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{302D1D41-67C7-48CF-B669-F1405844081C}" name="ID" dataDxfId="78"/>
-    <tableColumn id="10" xr3:uid="{DAC69B5A-FDB9-4E40-B9DF-D627D52F7026}" name="Order" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{18D1895A-6B8F-4769-905A-7B17388B3841}" name="Name" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{E78EEE3A-A310-4C93-BB56-91C774378558}" name="Description" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{C2498D1A-0522-4022-9828-720277BAEFA0}" name="Value" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{BB71E515-13E4-4082-A3A1-D5CF11AB41BF}" name="Dev stage" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{0A7A2F02-9DDB-46CC-B9E9-6F4043AA6C8E}" name="Dev name" dataDxfId="72"/>
-    <tableColumn id="8" xr3:uid="{1A01A450-5656-4140-92D1-0B7B3AD63520}" name="Summary" dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{A56D811E-456F-4EB8-84F6-7E60D2DC5AE0}" name="Notes" dataDxfId="70"/>
-    <tableColumn id="9" xr3:uid="{C5903060-FD83-4888-9AFB-276905D2A13A}" name="Dev stage order" dataDxfId="69">
+    <tableColumn id="1" xr3:uid="{302D1D41-67C7-48CF-B669-F1405844081C}" name="ID" dataDxfId="111"/>
+    <tableColumn id="10" xr3:uid="{DAC69B5A-FDB9-4E40-B9DF-D627D52F7026}" name="Order" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{18D1895A-6B8F-4769-905A-7B17388B3841}" name="Name" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{E78EEE3A-A310-4C93-BB56-91C774378558}" name="Description" dataDxfId="108"/>
+    <tableColumn id="5" xr3:uid="{C2498D1A-0522-4022-9828-720277BAEFA0}" name="Value" dataDxfId="107"/>
+    <tableColumn id="6" xr3:uid="{BB71E515-13E4-4082-A3A1-D5CF11AB41BF}" name="Dev stage" dataDxfId="106"/>
+    <tableColumn id="7" xr3:uid="{0A7A2F02-9DDB-46CC-B9E9-6F4043AA6C8E}" name="Dev name" dataDxfId="105"/>
+    <tableColumn id="8" xr3:uid="{1A01A450-5656-4140-92D1-0B7B3AD63520}" name="Summary" dataDxfId="104"/>
+    <tableColumn id="11" xr3:uid="{A56D811E-456F-4EB8-84F6-7E60D2DC5AE0}" name="Notes" dataDxfId="103"/>
+    <tableColumn id="9" xr3:uid="{C5903060-FD83-4888-9AFB-276905D2A13A}" name="Dev stage order" dataDxfId="102">
       <calculatedColumnFormula>VLOOKUP(TableAttack[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1620,27 +1606,27 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
   <autoFilter ref="A1:O2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O2">
     <sortCondition descending="1" ref="D1:D2"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="118"/>
-    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="117"/>
-    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="116"/>
-    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="115"/>
-    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="114"/>
-    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="113"/>
-    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="112"/>
-    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="111"/>
-    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="110"/>
-    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="109"/>
-    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="108"/>
-    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="107">
+    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="96"/>
+    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="95"/>
+    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="94"/>
+    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="93"/>
+    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="92"/>
+    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="91"/>
+    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="90"/>
+    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="89"/>
+    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="88"/>
+    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="87"/>
+    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="86"/>
+    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="85">
       <calculatedColumnFormula>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1994,7 +1980,7 @@
   <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2045,7 @@
         <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>79</v>
@@ -2080,13 +2066,13 @@
         <v>91</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>81</v>
@@ -2122,7 +2108,7 @@
         <v>48</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>89</v>
@@ -2218,9 +2204,9 @@
       <c r="S2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T2" s="1" t="e">
+      <c r="T2" s="1">
         <f>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</f>
-        <v>#REF!</v>
+        <v>35</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2" t="s">
@@ -2241,7 +2227,7 @@
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AF2" s="1" t="e">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</f>
@@ -2256,8 +2242,8 @@
         <v>#N/A</v>
       </c>
       <c r="AI2" s="1" t="e">
-        <f>IF(ISBLANK(#REF!),0,VLOOKUP(#REF!,TableValueAtk[],2,FALSE))</f>
-        <v>#REF!</v>
+        <f>IF(ISBLANK(TableCreature[[#This Row],[Atk Str]]),0,VLOOKUP(TableCreature[[#This Row],[Atk Str]],TableValueAtk[],2,FALSE))</f>
+        <v>#N/A</v>
       </c>
       <c r="AJ2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</f>
@@ -2287,52 +2273,47 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2 K2:N2 AF2:AO2">
-    <cfRule type="expression" dxfId="68" priority="13">
+  <conditionalFormatting sqref="A2 AF2:AO2 K2:O2">
+    <cfRule type="expression" dxfId="68" priority="14">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="67" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="5" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="6" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="7" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="8" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="9" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="10" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="13" operator="equal">
       <formula>"Yellow"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2">
+    <cfRule type="expression" dxfId="56" priority="2">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2">
-    <cfRule type="expression" dxfId="58" priority="3">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="56" priority="2">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2">
-    <cfRule type="expression" dxfId="55" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2466,41 +2447,41 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="54" priority="11">
+    <cfRule type="expression" dxfId="55" priority="11">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="53" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="8" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="9" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="44" priority="1">
+    <cfRule type="expression" dxfId="45" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2526,8 +2507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EDC1F1-8E32-4E12-A5F3-D0E3A339A822}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,12 +2599,12 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="43" priority="2">
+    <cfRule type="expression" dxfId="44" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="expression" dxfId="42" priority="1">
+    <cfRule type="expression" dxfId="43" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2647,7 +2628,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,16 +2679,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E2" s="2">
         <v>10</v>
@@ -2716,10 +2697,10 @@
         <v>72</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="1">
@@ -2729,12 +2710,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="39" priority="2">
+    <cfRule type="expression" dxfId="42" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="expression" dxfId="38" priority="1">
+    <cfRule type="expression" dxfId="41" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2874,140 +2855,140 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="37" priority="56">
+    <cfRule type="expression" dxfId="40" priority="56">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="36" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="27" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="26" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="25" operator="equal">
       <formula>"XXX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
-      <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
-      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:L1">
-    <cfRule type="cellIs" dxfId="33" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+      <formula>"Yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
+      <formula>"Orange"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
+      <formula>"Green"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+      <formula>"Blue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+      <formula>"White"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+      <formula>"Purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+      <formula>"Pink"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+      <formula>"Black"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>"Cyan"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
-      <formula>"Black"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
-      <formula>"Pink"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
-      <formula>"Purple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
-      <formula>"White"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="33" operator="equal">
-      <formula>"Blue"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="43" operator="equal">
-      <formula>"Green"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="44" operator="equal">
-      <formula>"Orange"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="45" operator="equal">
-      <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
-      <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>"XXX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
-      <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
-      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
       <formula>"XXX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
-      <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
-      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"XXX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
-      <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
-      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"XXX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"XXX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
-      <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
-      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"XXX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"XX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"XXX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"XX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="0" priority="46">
+    <cfRule type="expression" dxfId="3" priority="46">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implement strong and technical attacks (#18)
* Implement attack core classes

* Add strong and technical attacks to creature core class

* Fix bugs

* Update creatures data to new format

* Uniform creature data

* Remove export from example

* Rename value --> variable for creature attacks

* Add attacks to utils

* Fix path

* Fix name

* Add import

* Fix yaml export format

* Update to include attacks

* Add first attack effect

* Fix yaml format

* Add export of attacks to color overview

* Fix yaml field name

* Fix yaml extraction

* Change colum order

* Update colors

* Fix atk reference

* Update .exe
</commit_message>
<xml_diff>
--- a/excel_base.xlsx
+++ b/excel_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\PycharmProjects\yacg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04734AA-FE71-47A2-93B9-481C02AF2E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5181970C-CAB2-4D31-8AD5-6BAD4F69F2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="570" windowWidth="29040" windowHeight="15720" xr2:uid="{F093FBEA-529F-4B59-A3F4-BB86ECC0062F}"/>
   </bookViews>
@@ -16,18 +16,19 @@
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
     <sheet name="Effects" sheetId="4" r:id="rId2"/>
     <sheet name="Traits" sheetId="3" r:id="rId3"/>
-    <sheet name="Colors Overview" sheetId="6" r:id="rId4"/>
-    <sheet name="Creatures - Value" sheetId="2" r:id="rId5"/>
-    <sheet name="Misc" sheetId="5" r:id="rId6"/>
+    <sheet name="Attacks" sheetId="7" r:id="rId4"/>
+    <sheet name="Colors Overview" sheetId="6" r:id="rId5"/>
+    <sheet name="Creatures - Value" sheetId="2" r:id="rId6"/>
+    <sheet name="Misc" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="ListColor" localSheetId="3">TableColor[Color]</definedName>
+    <definedName name="ListColor" localSheetId="4">TableColor[Color]</definedName>
     <definedName name="ListColor">TableColor[Color]</definedName>
-    <definedName name="ListDevStage" localSheetId="3">TableDevStage[Dev stage]</definedName>
+    <definedName name="ListDevStage" localSheetId="4">TableDevStage[Dev stage]</definedName>
     <definedName name="ListDevStage">TableDevStage[Dev stage]</definedName>
-    <definedName name="ListEffectType" localSheetId="3">TableEffectType[Effect type]</definedName>
+    <definedName name="ListEffectType" localSheetId="4">TableEffectType[Effect type]</definedName>
     <definedName name="ListEffectType">TableEffectType[Effect type]</definedName>
-    <definedName name="ListTraitType" localSheetId="3">TableTraitType[Trait type]</definedName>
+    <definedName name="ListTraitType" localSheetId="4">TableTraitType[Trait type]</definedName>
     <definedName name="ListTraitType">TableTraitType[Trait type]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -182,9 +183,6 @@
     <t>Showcase trait YAML</t>
   </si>
   <si>
-    <t>TXXX</t>
-  </si>
-  <si>
     <t>Template creature</t>
   </si>
   <si>
@@ -321,16 +319,61 @@
   </si>
   <si>
     <t>MEC-XXX</t>
+  </si>
+  <si>
+    <t>ID Atk Tec</t>
+  </si>
+  <si>
+    <t>Atk Str</t>
+  </si>
+  <si>
+    <t>Atk Str Effect</t>
+  </si>
+  <si>
+    <t>Atk Tec</t>
+  </si>
+  <si>
+    <t>Atk Tec Effect</t>
+  </si>
+  <si>
+    <t>ATT-XXX</t>
+  </si>
+  <si>
+    <t>Cookie Monster</t>
+  </si>
+  <si>
+    <t>Eat an Oreo</t>
+  </si>
+  <si>
+    <t>Template attack</t>
+  </si>
+  <si>
+    <t>Showcase attack YAML</t>
+  </si>
+  <si>
+    <t>ID Atk Str</t>
+  </si>
+  <si>
+    <t>Atk Str Effect Variable</t>
+  </si>
+  <si>
+    <t>Atk Tec Effect Variable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -398,7 +441,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="159">
+  <dxfs count="182">
     <dxf>
       <fill>
         <patternFill patternType="lightDown">
@@ -700,6 +743,20 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
@@ -773,6 +830,20 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
@@ -995,6 +1066,51 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1149,6 +1265,42 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -1162,14 +1314,6 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1238,72 +1382,83 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="158" dataDxfId="157">
-  <autoFilter ref="A1:AH2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
-  <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="156"/>
-    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="155"/>
-    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="154"/>
-    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="153"/>
-    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="152"/>
-    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="151"/>
-    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="150"/>
-    <tableColumn id="6" xr3:uid="{C656462A-1289-4B31-94BD-E92D708B3664}" name="Atk" dataDxfId="149"/>
-    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="148"/>
-    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="147">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}" name="TableCreature" displayName="TableCreature" ref="A1:AO2" totalsRowShown="0" headerRowDxfId="181" dataDxfId="180">
+  <autoFilter ref="A1:AO2" xr:uid="{2D76BCAE-74FE-478B-9832-C5C15E51EB33}"/>
+  <tableColumns count="41">
+    <tableColumn id="1" xr3:uid="{3BBCBF5E-378C-4BAD-81D7-D4058E99F768}" name="ID" dataDxfId="179"/>
+    <tableColumn id="33" xr3:uid="{313F0E84-915A-4BBC-9519-B648F703BCEC}" name="Order" dataDxfId="178"/>
+    <tableColumn id="28" xr3:uid="{00B5C22B-51CF-490D-9627-D8EC73369F68}" name="Name" dataDxfId="177"/>
+    <tableColumn id="2" xr3:uid="{799BBE31-D9CF-4B3F-A4AD-2A368F9C40F1}" name="Color" dataDxfId="176"/>
+    <tableColumn id="3" xr3:uid="{82D500DC-2DFE-4C11-B15F-327CA5B3538B}" name="Cost (total)" dataDxfId="175"/>
+    <tableColumn id="4" xr3:uid="{55ED7849-5BAA-4141-88E9-32A0D1F6A14F}" name="Cost (color)" dataDxfId="174"/>
+    <tableColumn id="5" xr3:uid="{110A53AA-49BC-479E-AD44-A5F6ECFBA25B}" name="HP" dataDxfId="173"/>
+    <tableColumn id="7" xr3:uid="{6A940D9F-6AAB-4F26-8F83-328CFA37EC6A}" name="Spe" dataDxfId="172"/>
+    <tableColumn id="8" xr3:uid="{FBDDED27-7A6E-426C-93C2-6992272711C4}" name="Trait 1" dataDxfId="171">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="146">
+    <tableColumn id="9" xr3:uid="{C6FB2070-2D95-495D-B125-683FEC4BAE06}" name="Trait 2" dataDxfId="170">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="145">
+    <tableColumn id="10" xr3:uid="{948715A8-81EE-4457-BA20-05C1C909F8F3}" name="Trait 3" dataDxfId="169">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="144">
+    <tableColumn id="11" xr3:uid="{AC1B891A-F367-4E62-91F4-DAB7AD03F624}" name="Trait 4" dataDxfId="168">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8477F325-1B6C-4F6F-96EA-19C8F1B2CF75}" name="Value" dataDxfId="143">
+    <tableColumn id="6" xr3:uid="{424BC364-A4F7-4DFE-8B80-8C12E0214FC3}" name="Atk Str" dataDxfId="167"/>
+    <tableColumn id="42" xr3:uid="{FCE8FFB0-A25C-4332-9148-D1E698B1141E}" name="Atk Str Effect" dataDxfId="166">
+      <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Str]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="41" xr3:uid="{57099D6D-D357-433A-9C7B-03B59203392F}" name="Atk Str Effect Variable" dataDxfId="165"/>
+    <tableColumn id="12" xr3:uid="{C149A631-5763-43F0-BB5E-8DFC5A2DB802}" name="Atk Tec" dataDxfId="164"/>
+    <tableColumn id="43" xr3:uid="{A46124C8-35A4-4A34-AAA7-C77DEF20B192}" name="Atk Tec Effect" dataDxfId="163">
+      <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Tec]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="37" xr3:uid="{DDB782B7-3741-45E7-A296-44516E8DD74A}" name="Atk Tec Effect Variable" dataDxfId="162"/>
+    <tableColumn id="45" xr3:uid="{099F84C7-585A-4B39-97A1-6BA6794D5145}" name="Token?" dataDxfId="161"/>
+    <tableColumn id="48" xr3:uid="{6E8597CE-3227-4CD4-9431-F586DF7BB02D}" name="Value" dataDxfId="160">
       <calculatedColumnFormula>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{BACC1723-355A-4BD3-BEC6-02BFB69F5C34}" name="Token?" dataDxfId="142"/>
-    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="141"/>
-    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="140"/>
-    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="139"/>
-    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="138"/>
-    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="137"/>
-    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="136"/>
-    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="135"/>
-    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="134"/>
-    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="133"/>
-    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="132">
+    <tableColumn id="27" xr3:uid="{977ABA26-B008-44B5-9958-EC13499C30D6}" name="Flavor text" dataDxfId="159"/>
+    <tableColumn id="36" xr3:uid="{32A4983D-CE06-4C53-B9F4-4F5C256273FC}" name="Dev stage" dataDxfId="158"/>
+    <tableColumn id="24" xr3:uid="{6C7CBFA3-A00F-4B72-98E1-A0C45EE7DEE0}" name="Dev name" dataDxfId="157"/>
+    <tableColumn id="26" xr3:uid="{AFB64E65-D333-428F-94DC-B29188BCD29A}" name="Summary" dataDxfId="156"/>
+    <tableColumn id="25" xr3:uid="{548971E5-3054-4485-ADC2-E38ACCCF844C}" name="Notes" dataDxfId="155"/>
+    <tableColumn id="29" xr3:uid="{501C170F-AD76-4619-983F-CB5D2C889C06}" name="ID Trait 1" dataDxfId="154"/>
+    <tableColumn id="30" xr3:uid="{04CAA09B-DFE3-4A81-AF8D-EF71FF610434}" name="ID Trait 2" dataDxfId="153"/>
+    <tableColumn id="31" xr3:uid="{A03E6C45-456F-41EB-A187-77142E4E6D74}" name="ID Trait 3" dataDxfId="152"/>
+    <tableColumn id="32" xr3:uid="{D62F1380-6632-42CD-BF66-918AD91AD1B6}" name="ID Trait 4" dataDxfId="151"/>
+    <tableColumn id="39" xr3:uid="{6B1B591C-CE53-4B4A-9C9C-F299189689D7}" name="ID Atk Str" dataDxfId="150"/>
+    <tableColumn id="40" xr3:uid="{8B59C247-B367-4385-830E-BA42AF90CC0C}" name="ID Atk Tec" dataDxfId="149"/>
+    <tableColumn id="13" xr3:uid="{3A527FE0-AB3F-4AFF-9F13-6B0030250852}" name="[V] Color" dataDxfId="148">
       <calculatedColumnFormula>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="131">
+    <tableColumn id="14" xr3:uid="{12B3FD0A-7CC1-4991-B4ED-A1C56602FC6A}" name="[V] Cost (total)" dataDxfId="147">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,VLOOKUP(TableCreature[[#This Row],[Cost (total)]],TableValueCost[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="130">
+    <tableColumn id="15" xr3:uid="{DB2515AC-6885-43E3-B37A-991A940DF9A2}" name="[V] HP" dataDxfId="146">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[HP]]),0,VLOOKUP(TableCreature[[#This Row],[HP]],TableValueHP[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="129">
-      <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Atk]]),0,VLOOKUP(TableCreature[[#This Row],[Atk]],TableValueAtk[],2,FALSE))</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{C58F86A9-FA47-4272-A037-26D457345897}" name="[V] Atk" dataDxfId="145">
+      <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Atk Str]]),0,VLOOKUP(TableCreature[[#This Row],[Atk Str]],TableValueAtk[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="128">
+    <tableColumn id="17" xr3:uid="{E8E041D6-A2D4-475D-85E1-60D8BB4217D1}" name="[V] Spd" dataDxfId="144">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="127">
+    <tableColumn id="18" xr3:uid="{9BD73F82-7482-40C9-AC42-26A3CB15A78A}" name="[V] Trait 1" dataDxfId="143">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="126">
+    <tableColumn id="19" xr3:uid="{36C13983-0CE7-4355-9480-4F88AB6C49FB}" name="[V] Trait 2" dataDxfId="142">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="125">
+    <tableColumn id="20" xr3:uid="{0E0D8BF5-05B9-4B3A-AEF7-630A5098CE38}" name="[V] Trait 3" dataDxfId="141">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="124">
+    <tableColumn id="21" xr3:uid="{D195A258-C26D-44D6-92ED-78E9E4A8F565}" name="[V] Trait 4" dataDxfId="140">
       <calculatedColumnFormula>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],6,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="123">
-      <calculatedColumnFormula>VLOOKUP(TableCreature[[#This Row],[Token?]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
+    <tableColumn id="22" xr3:uid="{FC3EA7BD-6DCA-4BC1-8063-FE74846E8866}" name="Dev stage order" dataDxfId="139">
+      <calculatedColumnFormula>VLOOKUP(TableCreature[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1311,70 +1466,81 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
-  <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
-    <sortCondition descending="1" ref="C1:C5"/>
-  </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}" name="TableValueSpd" displayName="TableValueSpd" ref="O1:P2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="O1:P2" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{70EAA4A7-45C8-47B4-B396-C1BB012C4459}" name="Spd"/>
+    <tableColumn id="2" xr3:uid="{D4251DEB-6809-4B65-9CDC-E6F699CEE4D1}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
-  <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}" name="TableDevStage" displayName="TableDevStage" ref="A1:C5" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+  <autoFilter ref="A1:C5" xr:uid="{D01B2D53-F070-4BFA-8676-CFB92BCE9592}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
+    <sortCondition descending="1" ref="C1:C5"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{AAC98F6E-12C3-4B31-A187-477518FA3B90}" name="Dev stage" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{61F0B933-B445-4B79-9C9E-FD3260C28587}" name="Description" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{2466C595-18A9-4B05-9833-5913053554D4}" name="Order" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
-  <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}" name="TableColor" displayName="TableColor" ref="E1:E11" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+  <autoFilter ref="E1:E11" xr:uid="{6A2D9144-858C-458E-BEEA-4653BCBA1BC7}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{2553E31B-3CDD-4AD0-8BAF-B2E9A1742DA2}" name="Color" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}" name="TableTraitType" displayName="TableTraitType" ref="J1:K4" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+  <autoFilter ref="J1:K4" xr:uid="{B0D19AFC-73D7-473B-A70A-E4B7467B7E5E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6699292C-6526-402E-AA0B-397C27CCFE48}" name="Trait type" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{35DF6400-FAEA-4190-8EE7-7400449B69BC}" name="Description" dataDxfId="69"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}" name="TableEffectType" displayName="TableEffectType" ref="G1:H4" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="G1:H4" xr:uid="{35A653F1-009B-4829-B13D-8E96506814F1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{F360F71D-9E4C-4C2F-B5C9-6CB049721F2C}" name="Effect type" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{B7E0816B-0920-41FA-961E-DA4A17B5A9A0}" name="Description" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}" name="TableEffect" displayName="TableEffect" ref="A1:N2" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137">
   <autoFilter ref="A1:N2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="113"/>
-    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="112"/>
-    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="111"/>
-    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="110"/>
-    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="109"/>
-    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="108"/>
-    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="107">
+    <tableColumn id="1" xr3:uid="{76DBBEA2-63FD-4A97-AEA2-FC8C904F3300}" name="ID" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{06B0666D-5AF0-402A-9EC6-B45A74684D95}" name="Order" dataDxfId="135"/>
+    <tableColumn id="3" xr3:uid="{B4154627-4E71-4574-893E-CD960C167A57}" name="Name" dataDxfId="134"/>
+    <tableColumn id="4" xr3:uid="{0320F865-92F7-4AF2-BC3E-EE2C4B82F212}" name="Color" dataDxfId="133"/>
+    <tableColumn id="5" xr3:uid="{03950D48-2605-4EE2-B498-D544296D9E7B}" name="Type" dataDxfId="132"/>
+    <tableColumn id="6" xr3:uid="{AEF463B5-6CE0-4693-A266-BC4C4022FB8A}" name="Cost (total)" dataDxfId="131"/>
+    <tableColumn id="7" xr3:uid="{75001AE0-C177-4809-B283-95F0969C8D08}" name="Cost (color)" dataDxfId="130"/>
+    <tableColumn id="8" xr3:uid="{E6D16330-B913-42EC-AF38-6B98259C6362}" name="Description" dataDxfId="129"/>
+    <tableColumn id="14" xr3:uid="{E17355B6-35A6-413C-BD4E-38AA44182BB8}" name="Flavor text" dataDxfId="128"/>
+    <tableColumn id="9" xr3:uid="{4A5F95E3-BFE7-4998-93C0-287C296DD3AE}" name="Dev stage" dataDxfId="127"/>
+    <tableColumn id="10" xr3:uid="{30F52C15-0ECD-4E84-9B65-D2CA768B7802}" name="Dev name" dataDxfId="126"/>
+    <tableColumn id="11" xr3:uid="{9DE73668-4199-4C38-BE9A-3B0140A3E988}" name="Summary" dataDxfId="125"/>
+    <tableColumn id="13" xr3:uid="{5865281E-BD41-44CE-AF45-8907FA465354}" name="Notes" dataDxfId="124"/>
+    <tableColumn id="12" xr3:uid="{0A0A5A15-9C77-4A04-8ED3-2A1F2885688D}" name="Dev stage order" dataDxfId="123">
       <calculatedColumnFormula>VLOOKUP(TableEffect[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1383,20 +1549,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}" name="TableTrait" displayName="TableTrait" ref="A1:K2" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
   <autoFilter ref="A1:K2" xr:uid="{EEC7BFAF-2411-4A87-9C22-7CA9909BDCF3}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="104"/>
-    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="101"/>
-    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="99"/>
-    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="98"/>
-    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="97"/>
-    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="96"/>
-    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="95"/>
-    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="94">
+    <tableColumn id="1" xr3:uid="{EED6930E-6A92-46CD-A9D6-9ABCC5C6B23D}" name="ID" dataDxfId="120"/>
+    <tableColumn id="10" xr3:uid="{E9391A12-F7F3-4416-A5D6-E95077EB91FB}" name="Order" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{C1408B00-8940-4003-8815-490C013A634E}" name="Name" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{091F37F7-1CB9-402F-A1C1-5D78F1CEF94E}" name="Description" dataDxfId="117"/>
+    <tableColumn id="4" xr3:uid="{4D2BCFA2-D8C6-46AA-BA51-8DC3B333A3C3}" name="Type" dataDxfId="116"/>
+    <tableColumn id="5" xr3:uid="{D09E12CB-0986-4470-9BD9-08F84226DE2B}" name="Value" dataDxfId="115"/>
+    <tableColumn id="6" xr3:uid="{271C66C1-5D3C-45DA-9CF3-304C7ED9B65F}" name="Dev stage" dataDxfId="114"/>
+    <tableColumn id="7" xr3:uid="{8EB53856-2CBC-4DA3-B0CE-1DE45629F686}" name="Dev name" dataDxfId="113"/>
+    <tableColumn id="8" xr3:uid="{CBCFAE15-D602-497C-B122-B4335B3B8944}" name="Summary" dataDxfId="112"/>
+    <tableColumn id="11" xr3:uid="{088E13C1-2A25-4D0E-87BD-EB12A6B77927}" name="Notes" dataDxfId="111"/>
+    <tableColumn id="9" xr3:uid="{7217FFF8-D25F-4E64-BBDC-78425B1A4E00}" name="Dev stage order" dataDxfId="110">
       <calculatedColumnFormula>VLOOKUP(TableTrait[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1405,27 +1571,48 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0FD50C52-5470-4FA1-B963-FCCA8A3AEA14}" name="TableAttack" displayName="TableAttack" ref="A1:J2" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
+  <autoFilter ref="A1:J2" xr:uid="{0FD50C52-5470-4FA1-B963-FCCA8A3AEA14}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{302D1D41-67C7-48CF-B669-F1405844081C}" name="ID" dataDxfId="107"/>
+    <tableColumn id="10" xr3:uid="{DAC69B5A-FDB9-4E40-B9DF-D627D52F7026}" name="Order" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{18D1895A-6B8F-4769-905A-7B17388B3841}" name="Name" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{E78EEE3A-A310-4C93-BB56-91C774378558}" name="Description" dataDxfId="104"/>
+    <tableColumn id="5" xr3:uid="{C2498D1A-0522-4022-9828-720277BAEFA0}" name="Value" dataDxfId="103"/>
+    <tableColumn id="6" xr3:uid="{BB71E515-13E4-4082-A3A1-D5CF11AB41BF}" name="Dev stage" dataDxfId="102"/>
+    <tableColumn id="7" xr3:uid="{0A7A2F02-9DDB-46CC-B9E9-6F4043AA6C8E}" name="Dev name" dataDxfId="101"/>
+    <tableColumn id="8" xr3:uid="{1A01A450-5656-4140-92D1-0B7B3AD63520}" name="Summary" dataDxfId="100"/>
+    <tableColumn id="11" xr3:uid="{A56D811E-456F-4EB8-84F6-7E60D2DC5AE0}" name="Notes" dataDxfId="99"/>
+    <tableColumn id="9" xr3:uid="{C5903060-FD83-4888-9AFB-276905D2A13A}" name="Dev stage order" dataDxfId="98">
+      <calculatedColumnFormula>VLOOKUP(TableAttack[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{89290937-17AD-4314-BD79-D8074C96AEBC}" name="TableMechanic" displayName="TableMechanic" ref="A1:O2" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A1:O2" xr:uid="{6BC14CD1-4C72-49AB-903A-A9F4EC032073}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O2">
     <sortCondition descending="1" ref="D1:D2"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="88"/>
-    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="87"/>
-    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="86"/>
-    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="85"/>
-    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="84"/>
-    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="83"/>
-    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="82"/>
-    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="81"/>
-    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="80"/>
-    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="79"/>
-    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="78"/>
-    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="77">
+    <tableColumn id="1" xr3:uid="{68BB05F8-57DE-40CE-9D56-3AD020B647A2}" name="ID" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{01C11AC8-8958-447E-A33C-2A7AB069E4FF}" name="Order" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{9AC0759D-2EA2-4305-9F5F-CF6D6C3AA117}" name="Name" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{E813979E-35FC-4535-84BC-FBE7164018C9}" name="Orange" dataDxfId="92"/>
+    <tableColumn id="15" xr3:uid="{A5815C16-1C2D-420F-8652-4B3A49F22EEB}" name="Green" dataDxfId="91"/>
+    <tableColumn id="22" xr3:uid="{290A4B65-1FD1-4052-B37F-AF8EA313DA89}" name="Blue" dataDxfId="90"/>
+    <tableColumn id="21" xr3:uid="{78563779-9778-4BCF-8A4F-F97F9E6123B6}" name="White" dataDxfId="89"/>
+    <tableColumn id="20" xr3:uid="{2FF4C05C-93FB-4F1D-8832-EDECD2C6C8CE}" name="Yellow" dataDxfId="88"/>
+    <tableColumn id="19" xr3:uid="{C979B59C-F1E6-4032-9B88-39C51A731F36}" name="Purple" dataDxfId="87"/>
+    <tableColumn id="18" xr3:uid="{468177C3-A93C-4992-BFAB-11C7AAB0C780}" name="Pink" dataDxfId="86"/>
+    <tableColumn id="17" xr3:uid="{F1BC91B4-7E94-40CE-A153-07D3F6BF385E}" name="Black" dataDxfId="85"/>
+    <tableColumn id="16" xr3:uid="{B47320E9-E90C-49AE-AAEB-401F36E9CAF1}" name="Cyan" dataDxfId="84"/>
+    <tableColumn id="9" xr3:uid="{25B65F85-C5B5-4E80-956D-04080613CFC7}" name="Dev stage" dataDxfId="83"/>
+    <tableColumn id="13" xr3:uid="{BE42E863-EC00-46ED-BBD2-DE5331F0A01C}" name="Notes" dataDxfId="82"/>
+    <tableColumn id="12" xr3:uid="{ECDC8606-B3BA-4B17-B5DE-5DBC296871AD}" name="Dev stage order" dataDxfId="81">
       <calculatedColumnFormula>VLOOKUP(TableMechanic[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1433,7 +1620,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A3D9C3E-F2A3-44FB-A619-809AD2FF91C2}" name="TableValueCost" displayName="TableValueCost" ref="A1:B2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{0A3D9C3E-F2A3-44FB-A619-809AD2FF91C2}"/>
   <tableColumns count="2">
@@ -1444,7 +1631,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D43A2D6A-D008-4DB7-B5DD-C20DA025F23B}" name="TableValueColor" displayName="TableValueColor" ref="D1:G2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="D1:G2" xr:uid="{D43A2D6A-D008-4DB7-B5DD-C20DA025F23B}"/>
   <tableColumns count="4">
@@ -1457,7 +1644,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8B989991-971D-45B3-B881-5891B15ADD9B}" name="TableValueHP" displayName="TableValueHP" ref="I1:J2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="I1:J2" xr:uid="{8B989991-971D-45B3-B881-5891B15ADD9B}"/>
   <tableColumns count="2">
@@ -1468,23 +1655,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8CCFCB3C-4379-4941-93B9-2C56A7D66AA5}" name="TableValueAtk" displayName="TableValueAtk" ref="L1:M2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="L1:M2" xr:uid="{8CCFCB3C-4379-4941-93B9-2C56A7D66AA5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{038A2B11-8084-4C2F-A77A-AD359206B6A7}" name="Atk"/>
     <tableColumn id="2" xr3:uid="{1AF63558-B50E-4345-8ED8-AD5D661C3203}" name="Value"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}" name="TableValueSpd" displayName="TableValueSpd" ref="O1:P2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="O1:P2" xr:uid="{AB15239B-505B-492B-BF7C-B91CC45C0297}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{70EAA4A7-45C8-47B4-B396-C1BB012C4459}" name="Spd"/>
-    <tableColumn id="2" xr3:uid="{D4251DEB-6809-4B65-9CDC-E6F699CEE4D1}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1787,7 +1963,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB54C6D3-7FAB-4A2A-98C1-E20D603E5DF3}">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1801,28 +1977,35 @@
     <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" customWidth="1"/>
-    <col min="10" max="13" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="70.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="35.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="70.7109375" style="1" customWidth="1"/>
-    <col min="21" max="24" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="12" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="70.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="35.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="70.7109375" style="1" customWidth="1"/>
+    <col min="26" max="29" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1845,90 +2028,111 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>72</v>
+      <c r="AO1" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1949,133 +2153,161 @@
         <v>3</v>
       </c>
       <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2">
         <v>2</v>
       </c>
-      <c r="J2" s="1" t="e">
+      <c r="I2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],3,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K2" s="1" t="str">
+        <v>Subtle</v>
+      </c>
+      <c r="J2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],3,FALSE))</f>
         <v/>
       </c>
-      <c r="L2" s="1" t="str">
+      <c r="K2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],3,FALSE))</f>
         <v/>
       </c>
-      <c r="M2" s="1" t="str">
+      <c r="L2" s="1" t="str">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],3,FALSE))</f>
         <v/>
       </c>
-      <c r="N2" s="1">
+      <c r="M2" s="2">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1" t="str">
+        <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Str]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Str]],TableAttack[],3,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="str">
+        <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[ID Atk Tec]]),"",ISBLANK(VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE)),_xlfn.CONCAT("(",VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],8,FALSE),")"),TRUE,VLOOKUP(TableCreature[[#This Row],[ID Atk Tec]],TableAttack[],3,FALSE))</f>
+        <v>Cookie Monster</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
         <f>SUMIF(TableCreature[[#This Row],['[V'] Color]:['[V'] Trait 4]],"&lt;&gt;#N/A")</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="1" t="e">
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF2" s="1" t="e">
         <f>_xlfn.IFS(ISBLANK(TableCreature[[#This Row],[Color]]),0,ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,TableCreature[[#This Row],[Cost (total)]]&lt;3,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],2,FALSE),TableCreature[[#This Row],[Cost (total)]]&lt;6,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],3,FALSE),TRUE,VLOOKUP(TableCreature[[#This Row],[Color]],TableValueColor[],4,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="Z2" s="1" t="e">
+      <c r="AG2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[Cost (total)]]),0,VLOOKUP(TableCreature[[#This Row],[Cost (total)]],TableValueCost[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AA2" s="1" t="e">
+      <c r="AH2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[HP]]),0,VLOOKUP(TableCreature[[#This Row],[HP]],TableValueHP[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AB2" s="1" t="e">
-        <f>IF(ISBLANK(TableCreature[[#This Row],[Atk]]),0,VLOOKUP(TableCreature[[#This Row],[Atk]],TableValueAtk[],2,FALSE))</f>
+      <c r="AI2" s="1" t="e">
+        <f>IF(ISBLANK(TableCreature[[#This Row],[Atk Str]]),0,VLOOKUP(TableCreature[[#This Row],[Atk Str]],TableValueAtk[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AC2" s="1" t="e">
+      <c r="AJ2" s="1" t="e">
         <f>IF(ISBLANK(TableCreature[[#This Row],[Spe]]),0,VLOOKUP(TableCreature[[#This Row],[Spe]],TableValueSpd[],2,FALSE))</f>
         <v>#N/A</v>
       </c>
-      <c r="AD2" s="1" t="e">
+      <c r="AK2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 1]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 1]],TableTrait[],6,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AE2" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 2]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 2]],TableTrait[],6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AM2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 3]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 3]],TableTrait[],6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AN2" s="1">
         <f>IF(ISBLANK(TableCreature[[#This Row],[ID Trait 4]]),0,VLOOKUP(TableCreature[[#This Row],[ID Trait 4]],TableTrait[],6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AH2" s="1" t="e">
-        <f>VLOOKUP(TableCreature[[#This Row],[Token?]],TableDevStage[],3,FALSE)</f>
-        <v>#N/A</v>
+      <c r="AO2" s="1">
+        <f>VLOOKUP(TableCreature[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
-  <conditionalFormatting sqref="A2 J2:N2 Y2:AH2">
-    <cfRule type="expression" dxfId="60" priority="10">
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A2 I2:L2 N2 AF2:AO2">
+    <cfRule type="expression" dxfId="64" priority="14">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="5" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="6" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="7" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="8" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="11" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="12" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="13" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="Q2">
+    <cfRule type="expression" dxfId="54" priority="1">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2">
+    <cfRule type="expression" dxfId="53" priority="2">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{836D9E53-6903-4E55-A13E-DD3D2B77EB00}">
       <formula1>ListColor</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{C631AB10-2382-4312-BC45-9DB8F840C6A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2" xr:uid="{C631AB10-2382-4312-BC45-9DB8F840C6A5}">
       <formula1>ListDevStage</formula1>
     </dataValidation>
   </dataValidations>
@@ -2139,7 +2371,7 @@
         <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>21</v>
@@ -2151,27 +2383,27 @@
         <v>24</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2">
         <v>7</v>
@@ -2180,17 +2412,17 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="1">
@@ -2201,41 +2433,41 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="50" priority="11">
+    <cfRule type="expression" dxfId="52" priority="11">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
       <formula>"Cyan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="3" operator="equal">
       <formula>"Black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="4" operator="equal">
       <formula>"Pink"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="5" operator="equal">
       <formula>"Purple"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="6" operator="equal">
       <formula>"White"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="7" operator="equal">
       <formula>"Blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="8" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
       <formula>"Orange"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="40" priority="1">
+    <cfRule type="expression" dxfId="42" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2310,15 +2542,15 @@
         <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -2336,7 +2568,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>41</v>
@@ -2353,12 +2585,12 @@
   </sheetData>
   <sheetProtection insertRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="39" priority="2">
+    <cfRule type="expression" dxfId="41" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="expression" dxfId="38" priority="1">
+    <cfRule type="expression" dxfId="40" priority="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2378,6 +2610,114 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32583BC-C3F7-44B7-9986-764F4DA83BEC}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="9" max="9" width="70.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1">
+        <f>VLOOKUP(TableAttack[[#This Row],[Dev stage]],TableDevStage[],3,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="39" priority="2">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="expression" dxfId="38" priority="1">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{E870C36B-AC30-45BD-82C1-5939FB83ABBB}">
+      <formula1>ListDevStage</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9837E7-63C2-417A-ACE2-FDDEC9DFAE13}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2446,51 +2786,51 @@
         <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1">
@@ -2653,7 +2993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C196E161-DDDF-437F-9366-70D0E59EA547}">
   <dimension ref="A1:P1"/>
   <sheetViews>
@@ -2688,13 +3028,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>70</v>
-      </c>
-      <c r="G1" t="s">
-        <v>71</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2727,7 +3067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B963F87D-6D03-4FC0-968B-EAA63CF5DBB8}">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -2765,13 +3105,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>37</v>
@@ -2779,36 +3119,36 @@
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="3">
         <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3">
         <v>20</v>
@@ -2817,24 +3157,24 @@
         <v>29</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="3">
         <v>10</v>
@@ -2843,24 +3183,24 @@
         <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>

</xml_diff>